<commit_message>
Adjustments before testing on Raspi
</commit_message>
<xml_diff>
--- a/_analysis/_Results_compilation_training_flow_2024_06.xlsx
+++ b/_analysis/_Results_compilation_training_flow_2024_06.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Andre_Florentino\03_particular\04_mestrado-FEI\97_master\_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DC549A-A5FD-4A4D-B397-816BDFEC8D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D1D272-44F2-4CE7-BF9B-EEB35AFD8F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{765D2107-F650-4F10-ACE3-9E968F4DE976}"/>
   </bookViews>
@@ -643,11 +643,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -656,57 +656,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1656,15 +1606,15 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4266,15 +4216,15 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -5179,7 +5129,28 @@
     <dataField name="Average of recall" fld="4" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <conditionalFormats count="4">
-    <conditionalFormat priority="1">
+    <conditionalFormat priority="4">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="0" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="5">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="3">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -5187,7 +5158,7 @@
               <x v="1"/>
             </reference>
             <reference field="0" count="1" selected="0">
-              <x v="1"/>
+              <x v="0"/>
             </reference>
             <reference field="2" count="5">
               <x v="0"/>
@@ -5221,7 +5192,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="3">
+    <conditionalFormat priority="1">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -5229,28 +5200,7 @@
               <x v="1"/>
             </reference>
             <reference field="0" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="5">
-              <x v="0"/>
               <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="4">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="0" count="1" selected="0">
-              <x v="0"/>
             </reference>
             <reference field="2" count="5">
               <x v="0"/>
@@ -8046,7 +7996,211 @@
     <mergeCell ref="B23:B30"/>
     <mergeCell ref="D2:K2"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7 F7 H7 J7 L7 N7 P7 R7">
+  <conditionalFormatting sqref="D5 F5 H5 J5 L5 N5 P5 R5">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6 F6 H6 J6 L6 N6 P6 R6">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16 F16 H16 J16 L16 N16 P16 R16">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17 F17 H17 J17 L17 N17 P17 R17">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18 F18 H18 J18 L18 N18 P18 R18">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21 F21 H21 J21 L21 N21 P21 R21">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23 F23 H23 J23 L23 N23 P23 R23">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24 F24 H24 J24 L24 N24 P24 R24">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26 F26 H26 J26 L26 N26 P26 R26">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28 F28 H28 J28 L28 N28 P28 R28">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30 F30 H30 J30 L30 N30 P30 R30">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32 F32 H32 J32 L32 N32 P32 R32">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33 F33 H33 J33 L33 N33 P33 R33">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34 F34 H34 J34 L34 N34 P34 R34">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36 F36 H36 J36 L36 N36 P36 R36">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38 F38 H38 J38 L38 N38 P38 R38">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39 F39 H39 J39 L39 N39 P39 R39">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7 D7 H7 J7 L7 N7 P7 R7">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
@@ -8058,7 +8212,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8 F8 H8 J8 L8 N8 P8 R8">
+  <conditionalFormatting sqref="F8 D8 H8 J8 L8 N8 P8 R8">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -8070,7 +8224,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D9 F9 H9 J9 L9 N9 P9 R9">
+  <conditionalFormatting sqref="F9 D9 H9 J9 L9 N9 P9 R9">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -8082,7 +8236,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10 F10 H10 J10 L10 N10 P10 R10">
+  <conditionalFormatting sqref="F10 D10 H10 J10 L10 N10 P10 R10">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -8094,7 +8248,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11 F11 H11 J11 L11 N11 P11 R11">
+  <conditionalFormatting sqref="F11 D11 H11 J11 L11 N11 P11 R11">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -8106,7 +8260,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D12 F12 H12 J12 L12 N12 P12 R12">
+  <conditionalFormatting sqref="F12 D12 H12 J12 L12 N12 P12 R12">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -8118,7 +8272,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14 F14 H14 J14 L14 N14 P14 R14">
+  <conditionalFormatting sqref="F14 D14 H14 J14 L14 N14 P14 R14">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -8130,7 +8284,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15 F15 H15 J15 L15 N15 P15 R15">
+  <conditionalFormatting sqref="F15 D15 H15 J15 L15 N15 P15 R15">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -8142,7 +8296,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D19 F19 H19 J19 L19 N19 P19 R19">
+  <conditionalFormatting sqref="F19 D19 H19 J19 L19 N19 P19 R19">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -8154,7 +8308,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D20 F20 H20 J20 L20 N20 P20 R20">
+  <conditionalFormatting sqref="F20 D20 H20 J20 L20 N20 P20 R20">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -8166,7 +8320,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D25 F25 H25 J25 L25 N25 P25 R25">
+  <conditionalFormatting sqref="F25 D25 H25 J25 L25 N25 P25 R25">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -8178,7 +8332,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D27 F27 H27 J27 L27 N27 P27 R27">
+  <conditionalFormatting sqref="F27 D27 H27 J27 L27 N27 P27 R27">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -8190,7 +8344,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D29 F29 H29 J29 L29 N29 P29 R29">
+  <conditionalFormatting sqref="F29 D29 H29 J29 L29 N29 P29 R29">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -8202,7 +8356,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35 F35 H35 J35 L35 N35 P35 R35">
+  <conditionalFormatting sqref="F35 D35 H35 J35 L35 N35 P35 R35">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -8214,212 +8368,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37 F37 H37 J37 L37 N37 P37 R37">
+  <conditionalFormatting sqref="F37 D37 H37 J37 L37 N37 P37 R37">
     <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5 D5 H5 J5 L5 N5 P5 R5">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F6 D6 H6 J6 L6 N6 P6 R6">
-    <cfRule type="colorScale" priority="31">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F16 D16 H16 J16 L16 N16 P16 R16">
-    <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F17 D17 H17 J17 L17 N17 P17 R17">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F18 D18 H18 J18 L18 N18 P18 R18">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F21 D21 H21 J21 L21 N21 P21 R21">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F23 D23 H23 J23 L23 N23 P23 R23">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F24 D24 H24 J24 L24 N24 P24 R24">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F26 D26 H26 J26 L26 N26 P26 R26">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F28 D28 H28 J28 L28 N28 P28 R28">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F30 D30 H30 J30 L30 N30 P30 R30">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F32 D32 H32 J32 L32 N32 P32 R32">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F33 D33 H33 J33 L33 N33 P33 R33">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F34 D34 H34 J34 L34 N34 P34 R34">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F36 D36 H36 J36 L36 N36 P36 R36">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F38 D38 H38 J38 L38 N38 P38 R38">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F39 D39 H39 J39 L39 N39 P39 R39">
-    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -8680,7 +8630,7 @@
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B5" s="54" t="str">
+      <c r="B5" s="55" t="str">
         <f>IF(Aug_overview_classifier!B5=0,"",Aug_overview_classifier!B5)</f>
         <v>ESC10</v>
       </c>
@@ -9408,14 +9358,14 @@
         <f>IF(Aug_overview_classifier!S13=0,"",Aug_overview_classifier!S13)</f>
         <v/>
       </c>
-      <c r="U13" s="55">
+      <c r="U13" s="54">
         <f>AVERAGE(U5:V12)</f>
         <v>9.931847414804941E-3</v>
       </c>
-      <c r="V13" s="55"/>
+      <c r="V13" s="54"/>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B14" s="54" t="str">
+      <c r="B14" s="55" t="str">
         <f>IF(Aug_overview_classifier!B14=0,"",Aug_overview_classifier!B14)</f>
         <v>BDLib2</v>
       </c>
@@ -10143,14 +10093,14 @@
         <f>IF(Aug_overview_classifier!S22=0,"",Aug_overview_classifier!S22)</f>
         <v/>
       </c>
-      <c r="U22" s="55">
+      <c r="U22" s="54">
         <f>AVERAGE(U14:V21)</f>
         <v>5.9056245465618183E-2</v>
       </c>
-      <c r="V22" s="55"/>
+      <c r="V22" s="54"/>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B23" s="54" t="str">
+      <c r="B23" s="55" t="str">
         <f>IF(Aug_overview_classifier!B23=0,"",Aug_overview_classifier!B23)</f>
         <v>US8K</v>
       </c>
@@ -10878,14 +10828,14 @@
         <f>IF(Aug_overview_classifier!S31=0,"",Aug_overview_classifier!S31)</f>
         <v/>
       </c>
-      <c r="U31" s="55">
+      <c r="U31" s="54">
         <f>AVERAGE(U23:V30)</f>
         <v>-1.4491331682895237E-2</v>
       </c>
-      <c r="V31" s="55"/>
+      <c r="V31" s="54"/>
     </row>
     <row r="32" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B32" s="54" t="str">
+      <c r="B32" s="55" t="str">
         <f>IF(Aug_overview_classifier!B32=0,"",Aug_overview_classifier!B32)</f>
         <v>US8K_AV</v>
       </c>
@@ -11541,24 +11491,24 @@
       </c>
     </row>
     <row r="40" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="U40" s="55">
+      <c r="U40" s="54">
         <f>AVERAGE(U32:V39)</f>
         <v>-1.0395255911366967E-2</v>
       </c>
-      <c r="V40" s="55"/>
+      <c r="V40" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B32:B39"/>
+    <mergeCell ref="B5:B12"/>
+    <mergeCell ref="B14:B21"/>
+    <mergeCell ref="B23:B30"/>
     <mergeCell ref="U31:V31"/>
     <mergeCell ref="U22:V22"/>
     <mergeCell ref="U13:V13"/>
     <mergeCell ref="U40:V40"/>
     <mergeCell ref="D2:K2"/>
     <mergeCell ref="L2:S2"/>
-    <mergeCell ref="B32:B39"/>
-    <mergeCell ref="B5:B12"/>
-    <mergeCell ref="B14:B21"/>
-    <mergeCell ref="B23:B30"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D12 F5:F12 H5:H12 L5:L12 J5:J12 N5:N12 P5:P12 R5:R12">
     <cfRule type="colorScale" priority="7">
@@ -11609,12 +11559,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U5:V12 U14:V21 U23:V30">
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U32:V39">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14077,8 +14027,8 @@
     <mergeCell ref="B14:B21"/>
     <mergeCell ref="B23:B30"/>
   </mergeCells>
-  <conditionalFormatting sqref="D5 F5 H5 J5 L5 N5 P5 R5">
-    <cfRule type="colorScale" priority="40">
+  <conditionalFormatting sqref="D8 F8 H8 J8 L8 N8 P8 R8">
+    <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -14089,8 +14039,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6 F6 H6 J6 L6 N6 P6 R6">
-    <cfRule type="colorScale" priority="39">
+  <conditionalFormatting sqref="D10 F10 H10 J10 L10 N10 P10 R10">
+    <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -14101,8 +14051,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7 F7 H7 J7 L7 N7 P7 R7">
-    <cfRule type="colorScale" priority="38">
+  <conditionalFormatting sqref="D12 F12 H12 J12 L12 N12 P12 R12">
+    <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -14113,8 +14063,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D9 F9 H9 J9 L9 N9 P9 R9">
-    <cfRule type="colorScale" priority="36">
+  <conditionalFormatting sqref="D14 F14 H14 J14 L14 N14 P14 R14">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -14125,8 +14075,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11 F11 H11 J11 L11 N11 P11 R11">
-    <cfRule type="colorScale" priority="34">
+  <conditionalFormatting sqref="D15 F15 H15 J15 L15 N15 P15 R15">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -14137,8 +14087,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18 F18 H18 J18 L18 N18 P18 R18">
-    <cfRule type="colorScale" priority="28">
+  <conditionalFormatting sqref="D16 F16 H16 J16 L16 N16 P16 R16">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -14149,8 +14099,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D19 F19 H19 J19 L19 N19 P19 R19">
-    <cfRule type="colorScale" priority="27">
+  <conditionalFormatting sqref="D17 F17 H17 J17 L17 N17 P17 R17">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -14161,8 +14111,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D20 F20 H20 J20 L20 N20 P20 R20">
-    <cfRule type="colorScale" priority="26">
+  <conditionalFormatting sqref="D23 F23 H23 J23 L23 N23 P23 R23">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -14173,8 +14123,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D21 F21 H21 J21 L21 N21 P21 R21">
-    <cfRule type="colorScale" priority="25">
+  <conditionalFormatting sqref="D26 F26 H26 J26 L26 N26 P26 R26">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -14185,8 +14135,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D24 F24 H24 J24 L24 N24 P24 R24">
-    <cfRule type="colorScale" priority="23">
+  <conditionalFormatting sqref="D27 F27 H27 J27 L27 N27 P27 R27">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -14197,8 +14147,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D25 F25 H25 J25 L25 N25 P25 R25">
-    <cfRule type="colorScale" priority="22">
+  <conditionalFormatting sqref="D28 F28 H28 J28 L28 N28 P28 R28">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -14221,7 +14171,199 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37 F37 H37 J37 L37 N37 P37 R37">
+  <conditionalFormatting sqref="D32 F32 H32 J32 L32 N32 P32 R32">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33 F33 H33 J33 L33 N33 P33 R33">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34 F34 H34 J34 L34 N34 P34 R34">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35 F35 H35 J35 L35 N35 P35 R35">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36 F36 H36 J36 L36 N36 P36 R36">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5 D5 H5 J5 L5 N5 P5 R5">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6 D6 H6 J6 L6 N6 P6 R6">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7 D7 H7 J7 L7 N7 P7 R7">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9 D9 H9 J9 L9 N9 P9 R9">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11 D11 H11 J11 L11 N11 P11 R11">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18 D18 H18 J18 L18 N18 P18 R18">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F19 D19 H19 J19 L19 N19 P19 R19">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20 D20 H20 J20 L20 N20 P20 R20">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21 D21 H21 J21 L21 N21 P21 R21">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F24 D24 H24 J24 L24 N24 P24 R24">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F25 D25 H25 J25 L25 N25 P25 R25">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F37 D37 H37 J37 L37 N37 P37 R37">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -14233,7 +14375,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D38 F38 H38 J38 L38 N38 P38 R38">
+  <conditionalFormatting sqref="F38 D38 H38 J38 L38 N38 P38 R38">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -14245,200 +14387,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D39 F39 H39 J39 L39 N39 P39 R39">
+  <conditionalFormatting sqref="F39 D39 H39 J39 L39 N39 P39 R39">
     <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8 D8 H8 J8 L8 N8 P8 R8">
-    <cfRule type="colorScale" priority="37">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F10 D10 H10 J10 L10 N10 P10 R10">
-    <cfRule type="colorScale" priority="35">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12 D12 H12 J12 L12 N12 P12 R12">
-    <cfRule type="colorScale" priority="33">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F14 D14 H14 J14 L14 N14 P14 R14">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F15 D15 H15 J15 L15 N15 P15 R15">
-    <cfRule type="colorScale" priority="31">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F16 D16 H16 J16 L16 N16 P16 R16">
-    <cfRule type="colorScale" priority="30">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F17 D17 H17 J17 L17 N17 P17 R17">
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F23 D23 H23 J23 L23 N23 P23 R23">
-    <cfRule type="colorScale" priority="24">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F26 D26 H26 J26 L26 N26 P26 R26">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F27 D27 H27 J27 L27 N27 P27 R27">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F28 D28 H28 J28 L28 N28 P28 R28">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F32 D32 H32 J32 L32 N32 P32 R32">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F33 D33 H33 J33 L33 N33 P33 R33">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F34 D34 H34 J34 L34 N34 P34 R34">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F35 D35 H35 J35 L35 N35 P35 R35">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F36 D36 H36 J36 L36 N36 P36 R36">
-    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -14705,7 +14655,7 @@
       </c>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B5" s="54" t="str">
+      <c r="B5" s="55" t="str">
         <f>IF(Wind_overview_classifier!B5=0,"",Wind_overview_classifier!B5)</f>
         <v>ESC10</v>
       </c>
@@ -15497,19 +15447,19 @@
         <f>IF(Wind_overview_classifier!S13=0,"",Wind_overview_classifier!S13)</f>
         <v/>
       </c>
-      <c r="U13" s="55">
+      <c r="U13" s="54">
         <f>AVERAGE(U5:V12)</f>
         <v>-7.9568010334686051E-2</v>
       </c>
-      <c r="V13" s="55"/>
-      <c r="X13" s="55">
+      <c r="V13" s="54"/>
+      <c r="X13" s="54">
         <f>AVERAGE(X5:Y12)</f>
         <v>-6.9913669799093039E-2</v>
       </c>
-      <c r="Y13" s="55"/>
+      <c r="Y13" s="54"/>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B14" s="54" t="str">
+      <c r="B14" s="55" t="str">
         <f>IF(Wind_overview_classifier!B14=0,"",Wind_overview_classifier!B14)</f>
         <v>BDLib2</v>
       </c>
@@ -16301,19 +16251,19 @@
         <f>IF(Wind_overview_classifier!S22=0,"",Wind_overview_classifier!S22)</f>
         <v/>
       </c>
-      <c r="U22" s="55">
+      <c r="U22" s="54">
         <f>AVERAGE(U14:V21)</f>
         <v>-5.6429771014280435E-2</v>
       </c>
-      <c r="V22" s="55"/>
-      <c r="X22" s="55">
+      <c r="V22" s="54"/>
+      <c r="X22" s="54">
         <f>AVERAGE(X14:Y21)</f>
         <v>1.4009872496864445E-3</v>
       </c>
-      <c r="Y22" s="55"/>
+      <c r="Y22" s="54"/>
     </row>
     <row r="23" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B23" s="54" t="str">
+      <c r="B23" s="55" t="str">
         <f>IF(Wind_overview_classifier!B23=0,"",Wind_overview_classifier!B23)</f>
         <v>US8K</v>
       </c>
@@ -17105,19 +17055,19 @@
         <f>IF(Wind_overview_classifier!S31=0,"",Wind_overview_classifier!S31)</f>
         <v/>
       </c>
-      <c r="U31" s="55">
+      <c r="U31" s="54">
         <f>AVERAGE(U23:V30)</f>
         <v>-5.8828208236583648E-2</v>
       </c>
-      <c r="V31" s="55"/>
-      <c r="X31" s="55">
+      <c r="V31" s="54"/>
+      <c r="X31" s="54">
         <f>AVERAGE(X23:Y30)</f>
         <v>-7.2315381830499625E-2</v>
       </c>
-      <c r="Y31" s="55"/>
+      <c r="Y31" s="54"/>
     </row>
     <row r="32" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B32" s="54" t="str">
+      <c r="B32" s="55" t="str">
         <f>IF(Wind_overview_classifier!B32=0,"",Wind_overview_classifier!B32)</f>
         <v>US8K_AV</v>
       </c>
@@ -17837,16 +17787,16 @@
       </c>
     </row>
     <row r="40" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="U40" s="55">
+      <c r="U40" s="54">
         <f>AVERAGE(U32:V39)</f>
         <v>-3.7702393529234927E-2</v>
       </c>
-      <c r="V40" s="55"/>
-      <c r="X40" s="55">
+      <c r="V40" s="54"/>
+      <c r="X40" s="54">
         <f>AVERAGE(X32:Y39)</f>
         <v>-4.8202925208779057E-2</v>
       </c>
-      <c r="Y40" s="55"/>
+      <c r="Y40" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -17916,27 +17866,27 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U5:V12 U14:V21 U23:V30">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U32:V39">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X5:Y12">
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X14:Y21">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X23:Y30">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U32:V39">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Adjustments after the Raspiberry Pi analysis
</commit_message>
<xml_diff>
--- a/_analysis/_Results_compilation_training_flow_2024_06.xlsx
+++ b/_analysis/_Results_compilation_training_flow_2024_06.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Andre_Florentino\03_particular\04_mestrado-FEI\97_master\_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393B8B54-2838-4A40-B98A-DB26333763AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2DA3A8-68C6-4645-8329-E35ACA33D405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{765D2107-F650-4F10-ACE3-9E968F4DE976}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{765D2107-F650-4F10-ACE3-9E968F4DE976}"/>
   </bookViews>
   <sheets>
     <sheet name="Aug_overview_classifier" sheetId="1" r:id="rId1"/>
     <sheet name="Aug_overview_dataset" sheetId="2" r:id="rId2"/>
     <sheet name="Wind_overview_classifier" sheetId="3" r:id="rId3"/>
     <sheet name="Wind_overview_dataset" sheetId="5" r:id="rId4"/>
-    <sheet name="Precision_Recall" sheetId="6" r:id="rId5"/>
   </sheets>
   <externalReferences>
+    <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
@@ -27,7 +27,6 @@
     <externalReference r:id="rId10"/>
     <externalReference r:id="rId11"/>
     <externalReference r:id="rId12"/>
-    <externalReference r:id="rId13"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="24">
   <si>
     <t>Mean</t>
   </si>
@@ -444,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -596,6 +595,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4475,23 +4477,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C84E9B-02A8-4A6E-9A9C-4104E745268F}">
   <dimension ref="B2:S39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="11" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="16" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" style="16" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" style="16" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="11" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" style="16" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" customWidth="1"/>
+    <col min="16" max="16" width="10.6640625" style="16" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:19" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="12"/>
       <c r="C2" s="20" t="s">
         <v>14</v>
@@ -4531,7 +4533,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="2:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="35" t="s">
         <v>15</v>
       </c>
@@ -4577,7 +4579,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B4" s="24"/>
       <c r="C4" s="25"/>
       <c r="D4" s="26" t="s">
@@ -4629,7 +4631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B5" s="47" t="s">
         <v>6</v>
       </c>
@@ -4701,7 +4703,7 @@
         <v>2.7099354235848503E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B6" s="47"/>
       <c r="C6" s="4" t="s">
         <v>18</v>
@@ -4771,7 +4773,7 @@
         <v>8.0719421454814852E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B7" s="47"/>
       <c r="C7" s="4" t="s">
         <v>3</v>
@@ -4841,7 +4843,7 @@
         <v>5.7008771254956896E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B8" s="47"/>
       <c r="C8" s="4" t="s">
         <v>19</v>
@@ -4911,7 +4913,7 @@
         <v>5.659615711335883E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B9" s="47"/>
       <c r="C9" s="4" t="s">
         <v>17</v>
@@ -4981,7 +4983,7 @@
         <v>7.725768570181224E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B10" s="47"/>
       <c r="C10" s="4" t="s">
         <v>4</v>
@@ -5051,7 +5053,7 @@
         <v>4.5586456322026181E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B11" s="47"/>
       <c r="C11" s="4" t="s">
         <v>5</v>
@@ -5121,7 +5123,7 @@
         <v>4.183300132670377E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B12" s="48"/>
       <c r="C12" s="6" t="s">
         <v>20</v>
@@ -5191,7 +5193,7 @@
         <v>4.6770717334674264E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B13" s="30"/>
       <c r="C13" s="25"/>
       <c r="D13" s="26"/>
@@ -5211,7 +5213,7 @@
       <c r="R13" s="29"/>
       <c r="S13" s="34"/>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B14" s="47" t="s">
         <v>7</v>
       </c>
@@ -5283,7 +5285,7 @@
         <v>5.3575837561071885E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B15" s="47"/>
       <c r="C15" s="4" t="s">
         <v>18</v>
@@ -5353,7 +5355,7 @@
         <v>9.6225044864939862E-3</v>
       </c>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B16" s="47"/>
       <c r="C16" s="4" t="s">
         <v>3</v>
@@ -5423,7 +5425,7 @@
         <v>2.5458753860865761E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B17" s="47"/>
       <c r="C17" s="4" t="s">
         <v>19</v>
@@ -5493,7 +5495,7 @@
         <v>6.3098981620002811E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B18" s="47"/>
       <c r="C18" s="4" t="s">
         <v>17</v>
@@ -5563,7 +5565,7 @@
         <v>1.9245008972987331E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B19" s="47"/>
       <c r="C19" s="4" t="s">
         <v>4</v>
@@ -5633,7 +5635,7 @@
         <v>5.3575837561072148E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B20" s="47"/>
       <c r="C20" s="4" t="s">
         <v>5</v>
@@ -5703,7 +5705,7 @@
         <v>3.4694433324435663E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B21" s="48"/>
       <c r="C21" s="6" t="s">
         <v>20</v>
@@ -5773,7 +5775,7 @@
         <v>1.6666666666666496E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B22" s="30"/>
       <c r="C22" s="25"/>
       <c r="D22" s="26"/>
@@ -5793,7 +5795,7 @@
       <c r="R22" s="29"/>
       <c r="S22" s="34"/>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B23" s="47" t="s">
         <v>8</v>
       </c>
@@ -5865,7 +5867,7 @@
         <v>4.4362319217983379E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B24" s="47"/>
       <c r="C24" s="4" t="s">
         <v>18</v>
@@ -5935,7 +5937,7 @@
         <v>5.0363616429460974E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B25" s="47"/>
       <c r="C25" s="4" t="s">
         <v>3</v>
@@ -6005,7 +6007,7 @@
         <v>6.1554295024420218E-2</v>
       </c>
     </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B26" s="47"/>
       <c r="C26" s="4" t="s">
         <v>19</v>
@@ -6075,7 +6077,7 @@
         <v>2.962107369301108E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B27" s="47"/>
       <c r="C27" s="4" t="s">
         <v>17</v>
@@ -6145,7 +6147,7 @@
         <v>3.1220495989087861E-2</v>
       </c>
     </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B28" s="47"/>
       <c r="C28" s="4" t="s">
         <v>4</v>
@@ -6215,7 +6217,7 @@
         <v>3.5253353024031292E-2</v>
       </c>
     </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B29" s="47"/>
       <c r="C29" s="4" t="s">
         <v>5</v>
@@ -6285,7 +6287,7 @@
         <v>4.1853247574758473E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B30" s="48"/>
       <c r="C30" s="6" t="s">
         <v>20</v>
@@ -6355,7 +6357,7 @@
         <v>4.2097691385037841E-2</v>
       </c>
     </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B31" s="30"/>
       <c r="C31" s="25"/>
       <c r="D31" s="26"/>
@@ -6375,7 +6377,7 @@
       <c r="R31" s="29"/>
       <c r="S31" s="34"/>
     </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B32" s="47" t="s">
         <v>23</v>
       </c>
@@ -6447,7 +6449,7 @@
         <v>5.2680761025622622E-2</v>
       </c>
     </row>
-    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B33" s="47"/>
       <c r="C33" s="4" t="s">
         <v>18</v>
@@ -6517,7 +6519,7 @@
         <v>4.8661670511817759E-2</v>
       </c>
     </row>
-    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B34" s="47"/>
       <c r="C34" s="4" t="s">
         <v>3</v>
@@ -6587,7 +6589,7 @@
         <v>4.6344311238478736E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B35" s="47"/>
       <c r="C35" s="4" t="s">
         <v>19</v>
@@ -6657,7 +6659,7 @@
         <v>2.4772141992337307E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B36" s="47"/>
       <c r="C36" s="4" t="s">
         <v>17</v>
@@ -6727,7 +6729,7 @@
         <v>2.3219868574884551E-2</v>
       </c>
     </row>
-    <row r="37" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B37" s="47"/>
       <c r="C37" s="4" t="s">
         <v>4</v>
@@ -6797,7 +6799,7 @@
         <v>3.405096917308921E-2</v>
       </c>
     </row>
-    <row r="38" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B38" s="47"/>
       <c r="C38" s="4" t="s">
         <v>5</v>
@@ -6867,7 +6869,7 @@
         <v>2.9455118821827914E-2</v>
       </c>
     </row>
-    <row r="39" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B39" s="48"/>
       <c r="C39" s="6" t="s">
         <v>20</v>
@@ -6946,6 +6948,90 @@
     <mergeCell ref="B23:B30"/>
     <mergeCell ref="D2:K2"/>
   </mergeCells>
+  <conditionalFormatting sqref="D6 F6 H6 J6 L6 N6 P6 R6">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7 F7 H7 J7 L7 N7 P7 R7">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10 F10 H10 J10 L10 N10 P10 R10">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14 F14 H14 J14 L14 N14 P14 R14">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15 F15 H15 J15 L15 N15 P15 R15">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29 F29 H29 J29 L29 N29 P29 R29">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32 F32 H32 J32 L32 N32 P32 R32">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F5 D5 H5 J5 L5 N5 P5 R5">
     <cfRule type="colorScale" priority="32">
       <colorScale>
@@ -6958,8 +7044,44 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6 F6 H6 J6 L6 N6 P6 R6">
-    <cfRule type="colorScale" priority="31">
+  <conditionalFormatting sqref="F8 D8 H8 J8 L8 N8 P8 R8">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9 D9 H9 J9 L9 N9 P9 R9">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11 D11 H11 J11 L11 N11 P11 R11">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12 D12 H12 J12 L12 N12 P12 R12">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7006,6 +7128,30 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F19 D19 H19 J19 L19 N19 P19 R19">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20 D20 H20 J20 L20 N20 P20 R20">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F21 D21 H21 J21 L21 N21 P21 R21">
     <cfRule type="colorScale" priority="17">
       <colorScale>
@@ -7042,8 +7188,32 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F25 D25 H25 J25 L25 N25 P25 R25">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F26 D26 H26 J26 L26 N26 P26 R26">
     <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F27 D27 H27 J27 L27 N27 P27 R27">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7078,18 +7248,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32 F32 H32 J32 L32 N32 P32 R32">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F33 D33 H33 J33 L33 N33 P33 R33">
     <cfRule type="colorScale" priority="7">
       <colorScale>
@@ -7114,8 +7272,32 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F35 D35 H35 J35 L35 N35 P35 R35">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F36 D36 H36 J36 L36 N36 P36 R36">
     <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F37 D37 H37 J37 L37 N37 P37 R37">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7150,186 +7332,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7 F7 H7 J7 L7 N7 P7 R7">
-    <cfRule type="colorScale" priority="30">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8 D8 H8 J8 L8 N8 P8 R8">
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F9 D9 H9 J9 L9 N9 P9 R9">
-    <cfRule type="colorScale" priority="28">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D10 F10 H10 J10 L10 N10 P10 R10">
-    <cfRule type="colorScale" priority="27">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F11 D11 H11 J11 L11 N11 P11 R11">
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12 D12 H12 J12 L12 N12 P12 R12">
-    <cfRule type="colorScale" priority="25">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14 F14 H14 J14 L14 N14 P14 R14">
-    <cfRule type="colorScale" priority="24">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D15 F15 H15 J15 L15 N15 P15 R15">
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F19 D19 H19 J19 L19 N19 P19 R19">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F20 D20 H20 J20 L20 N20 P20 R20">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F25 D25 H25 J25 L25 N25 P25 R25">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F27 D27 H27 J27 L27 N27 P27 R27">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D29 F29 H29 J29 L29 N29 P29 R29">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F35 D35 H35 J35 L35 N35 P35 R35">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F37 D37 H37 J37 L37 N37 P37 R37">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7340,22 +7342,22 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="11" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="16" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" style="16" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" style="16" customWidth="1"/>
-    <col min="20" max="20" width="1.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="11" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" style="16" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" customWidth="1"/>
+    <col min="16" max="16" width="10.6640625" style="16" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" style="16" customWidth="1"/>
+    <col min="20" max="20" width="1.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:22" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:22" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="str">
         <f>IF(Aug_overview_classifier!B2=0,"",Aug_overview_classifier!B2)</f>
         <v/>
@@ -7429,7 +7431,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="2:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="35" t="str">
         <f>IF(Aug_overview_classifier!B3=0,"",Aug_overview_classifier!B3)</f>
         <v>Model</v>
@@ -7503,7 +7505,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B4" s="24" t="str">
         <f>IF(Aug_overview_classifier!B4=0,"",Aug_overview_classifier!B4)</f>
         <v/>
@@ -7577,7 +7579,7 @@
         <v>Std</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B5" s="53" t="str">
         <f>IF(Aug_overview_classifier!B5=0,"",Aug_overview_classifier!B5)</f>
         <v>ESC10</v>
@@ -7659,7 +7661,7 @@
         <v>2.3529411764705577E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B6" s="47" t="str">
         <f>IF(Aug_overview_classifier!B6=0,"",Aug_overview_classifier!B6)</f>
         <v/>
@@ -7741,7 +7743,7 @@
         <v>-2.8333333333333655E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B7" s="47" t="str">
         <f>IF(Aug_overview_classifier!B7=0,"",Aug_overview_classifier!B7)</f>
         <v/>
@@ -7823,7 +7825,7 @@
         <v>2.7874564459930085E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B8" s="47" t="str">
         <f>IF(Aug_overview_classifier!B8=0,"",Aug_overview_classifier!B8)</f>
         <v/>
@@ -7905,7 +7907,7 @@
         <v>1.293532338308423E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B9" s="47" t="str">
         <f>IF(Aug_overview_classifier!B9=0,"",Aug_overview_classifier!B9)</f>
         <v/>
@@ -7987,7 +7989,7 @@
         <v>-2.9154518950438302E-3</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B10" s="47" t="str">
         <f>IF(Aug_overview_classifier!B10=0,"",Aug_overview_classifier!B10)</f>
         <v/>
@@ -8069,7 +8071,7 @@
         <v>5.3140096618353727E-3</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B11" s="47" t="str">
         <f>IF(Aug_overview_classifier!B11=0,"",Aug_overview_classifier!B11)</f>
         <v/>
@@ -8151,7 +8153,7 @@
         <v>3.2630522088352931E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B12" s="48" t="str">
         <f>IF(Aug_overview_classifier!B12=0,"",Aug_overview_classifier!B12)</f>
         <v/>
@@ -8233,7 +8235,7 @@
         <v>4.5641025641025346E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B13" s="30" t="str">
         <f>IF(Aug_overview_classifier!B13=0,"",Aug_overview_classifier!B13)</f>
         <v/>
@@ -8312,7 +8314,7 @@
       </c>
       <c r="V13" s="52"/>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B14" s="53" t="str">
         <f>IF(Aug_overview_classifier!B14=0,"",Aug_overview_classifier!B14)</f>
         <v>BDLib2</v>
@@ -8394,7 +8396,7 @@
         <v>-5.7870370370370905E-3</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B15" s="47" t="str">
         <f>IF(Aug_overview_classifier!B15=0,"",Aug_overview_classifier!B15)</f>
         <v/>
@@ -8476,7 +8478,7 @@
         <v>-4.4000000000000372E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B16" s="47" t="str">
         <f>IF(Aug_overview_classifier!B16=0,"",Aug_overview_classifier!B16)</f>
         <v/>
@@ -8558,7 +8560,7 @@
         <v>6.8452380952381153E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B17" s="47" t="str">
         <f>IF(Aug_overview_classifier!B17=0,"",Aug_overview_classifier!B17)</f>
         <v/>
@@ -8640,7 +8642,7 @@
         <v>9.5238095238090459E-3</v>
       </c>
     </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B18" s="47" t="str">
         <f>IF(Aug_overview_classifier!B18=0,"",Aug_overview_classifier!B18)</f>
         <v/>
@@ -8722,7 +8724,7 @@
         <v>7.051282051282004E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B19" s="47" t="str">
         <f>IF(Aug_overview_classifier!B19=0,"",Aug_overview_classifier!B19)</f>
         <v/>
@@ -8804,7 +8806,7 @@
         <v>2.3114355231143913E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B20" s="47" t="str">
         <f>IF(Aug_overview_classifier!B20=0,"",Aug_overview_classifier!B20)</f>
         <v/>
@@ -8886,7 +8888,7 @@
         <v>0.17622950819672112</v>
       </c>
     </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B21" s="48" t="str">
         <f>IF(Aug_overview_classifier!B21=0,"",Aug_overview_classifier!B21)</f>
         <v/>
@@ -8968,7 +8970,7 @@
         <v>0.18303571428571397</v>
       </c>
     </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B22" s="30" t="str">
         <f>IF(Aug_overview_classifier!B22=0,"",Aug_overview_classifier!B22)</f>
         <v/>
@@ -9047,7 +9049,7 @@
       </c>
       <c r="V22" s="52"/>
     </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B23" s="53" t="str">
         <f>IF(Aug_overview_classifier!B23=0,"",Aug_overview_classifier!B23)</f>
         <v>US8K</v>
@@ -9129,7 +9131,7 @@
         <v>-1.6213829198711283E-3</v>
       </c>
     </row>
-    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B24" s="47" t="str">
         <f>IF(Aug_overview_classifier!B24=0,"",Aug_overview_classifier!B24)</f>
         <v/>
@@ -9211,7 +9213,7 @@
         <v>-6.9708096779339646E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B25" s="47" t="str">
         <f>IF(Aug_overview_classifier!B25=0,"",Aug_overview_classifier!B25)</f>
         <v/>
@@ -9293,7 +9295,7 @@
         <v>1.4505669218352057E-2</v>
       </c>
     </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B26" s="47" t="str">
         <f>IF(Aug_overview_classifier!B26=0,"",Aug_overview_classifier!B26)</f>
         <v/>
@@ -9375,7 +9377,7 @@
         <v>-1.4666102087111943E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B27" s="47" t="str">
         <f>IF(Aug_overview_classifier!B27=0,"",Aug_overview_classifier!B27)</f>
         <v/>
@@ -9457,7 +9459,7 @@
         <v>1.4307751856672102E-2</v>
       </c>
     </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B28" s="47" t="str">
         <f>IF(Aug_overview_classifier!B28=0,"",Aug_overview_classifier!B28)</f>
         <v/>
@@ -9539,7 +9541,7 @@
         <v>-1.9345565361934547E-3</v>
       </c>
     </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B29" s="47" t="str">
         <f>IF(Aug_overview_classifier!B29=0,"",Aug_overview_classifier!B29)</f>
         <v/>
@@ -9621,7 +9623,7 @@
         <v>-1.714759822894385E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B30" s="48" t="str">
         <f>IF(Aug_overview_classifier!B30=0,"",Aug_overview_classifier!B30)</f>
         <v/>
@@ -9703,7 +9705,7 @@
         <v>-1.128752492413998E-2</v>
       </c>
     </row>
-    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B31" s="30" t="str">
         <f>IF(Aug_overview_classifier!B31=0,"",Aug_overview_classifier!B31)</f>
         <v/>
@@ -9782,7 +9784,7 @@
       </c>
       <c r="V31" s="52"/>
     </row>
-    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B32" s="53" t="str">
         <f>IF(Aug_overview_classifier!B32=0,"",Aug_overview_classifier!B32)</f>
         <v>US8K_AV</v>
@@ -9864,7 +9866,7 @@
         <v>-2.6953488532588388E-4</v>
       </c>
     </row>
-    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B33" s="47" t="str">
         <f>IF(Aug_overview_classifier!B33=0,"",Aug_overview_classifier!B33)</f>
         <v/>
@@ -9946,7 +9948,7 @@
         <v>-6.5164732424990657E-2</v>
       </c>
     </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B34" s="47" t="str">
         <f>IF(Aug_overview_classifier!B34=0,"",Aug_overview_classifier!B34)</f>
         <v/>
@@ -10028,7 +10030,7 @@
         <v>1.2094980093515062E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B35" s="47" t="str">
         <f>IF(Aug_overview_classifier!B35=0,"",Aug_overview_classifier!B35)</f>
         <v/>
@@ -10110,7 +10112,7 @@
         <v>-1.6341243577944531E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B36" s="47" t="str">
         <f>IF(Aug_overview_classifier!B36=0,"",Aug_overview_classifier!B36)</f>
         <v/>
@@ -10192,7 +10194,7 @@
         <v>1.7515293515845798E-2</v>
       </c>
     </row>
-    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B37" s="47" t="str">
         <f>IF(Aug_overview_classifier!B37=0,"",Aug_overview_classifier!B37)</f>
         <v/>
@@ -10274,7 +10276,7 @@
         <v>-3.3792627557065469E-3</v>
       </c>
     </row>
-    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B38" s="47" t="str">
         <f>IF(Aug_overview_classifier!B38=0,"",Aug_overview_classifier!B38)</f>
         <v/>
@@ -10356,7 +10358,7 @@
         <v>-5.2653729105160973E-3</v>
       </c>
     </row>
-    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B39" s="48" t="str">
         <f>IF(Aug_overview_classifier!B39=0,"",Aug_overview_classifier!B39)</f>
         <v/>
@@ -10438,7 +10440,7 @@
         <v>1.3389813031775333E-2</v>
       </c>
     </row>
-    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:22" x14ac:dyDescent="0.3">
       <c r="U40" s="52">
         <f>AVERAGE(U32:V39)</f>
         <v>-1.0565448561979364E-2</v>
@@ -10524,23 +10526,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5498D750-A77C-4E1F-AC8E-4A19415168F1}">
   <dimension ref="B2:S39"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="11" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="16" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" style="16" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" style="16" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="11" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" style="16" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" customWidth="1"/>
+    <col min="16" max="16" width="10.6640625" style="16" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:19" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="12"/>
       <c r="C2" s="20" t="s">
         <v>14</v>
@@ -10566,7 +10568,7 @@
       <c r="R2" s="46"/>
       <c r="S2" s="46"/>
     </row>
-    <row r="3" spans="2:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="35" t="s">
         <v>15</v>
       </c>
@@ -10604,8 +10606,10 @@
       </c>
       <c r="S3" s="38"/>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B4" s="55" t="s">
+        <v>6</v>
+      </c>
       <c r="C4" s="25"/>
       <c r="D4" s="26" t="s">
         <v>0</v>
@@ -10656,7 +10660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B5" s="47" t="s">
         <v>6</v>
       </c>
@@ -10728,7 +10732,7 @@
         <v>3.6554510121453804E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B6" s="47"/>
       <c r="C6" s="4" t="s">
         <v>18</v>
@@ -10798,7 +10802,7 @@
         <v>4.3329907964490905E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B7" s="47"/>
       <c r="C7" s="4" t="s">
         <v>3</v>
@@ -10868,7 +10872,7 @@
         <v>4.4837729927308778E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B8" s="47"/>
       <c r="C8" s="4" t="s">
         <v>19</v>
@@ -10938,7 +10942,7 @@
         <v>3.0879404047152215E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B9" s="47"/>
       <c r="C9" s="4" t="s">
         <v>17</v>
@@ -11008,7 +11012,7 @@
         <v>2.6567681351349553E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B10" s="47"/>
       <c r="C10" s="4" t="s">
         <v>4</v>
@@ -11078,7 +11082,7 @@
         <v>2.9035289801220693E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B11" s="47"/>
       <c r="C11" s="4" t="s">
         <v>5</v>
@@ -11148,7 +11152,7 @@
         <v>3.4742663735967461E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B12" s="48"/>
       <c r="C12" s="6" t="s">
         <v>20</v>
@@ -11218,8 +11222,10 @@
         <v>3.2014566755899074E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="30"/>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B13" s="55" t="s">
+        <v>7</v>
+      </c>
       <c r="C13" s="25"/>
       <c r="D13" s="26"/>
       <c r="E13" s="31"/>
@@ -11238,7 +11244,7 @@
       <c r="R13" s="29"/>
       <c r="S13" s="34"/>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B14" s="47" t="s">
         <v>7</v>
       </c>
@@ -11310,7 +11316,7 @@
         <v>2.1166709549459383E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B15" s="47"/>
       <c r="C15" s="4" t="s">
         <v>18</v>
@@ -11380,7 +11386,7 @@
         <v>2.089825219249036E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B16" s="47"/>
       <c r="C16" s="4" t="s">
         <v>3</v>
@@ -11450,7 +11456,7 @@
         <v>1.3459823726881929E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B17" s="47"/>
       <c r="C17" s="4" t="s">
         <v>19</v>
@@ -11520,7 +11526,7 @@
         <v>1.1321681226052151E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B18" s="47"/>
       <c r="C18" s="4" t="s">
         <v>17</v>
@@ -11590,7 +11596,7 @@
         <v>2.1004350908505859E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B19" s="47"/>
       <c r="C19" s="4" t="s">
         <v>4</v>
@@ -11660,7 +11666,7 @@
         <v>1.7816473545345952E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B20" s="47"/>
       <c r="C20" s="4" t="s">
         <v>5</v>
@@ -11730,7 +11736,7 @@
         <v>9.4185790570313638E-3</v>
       </c>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B21" s="48"/>
       <c r="C21" s="6" t="s">
         <v>20</v>
@@ -11800,8 +11806,10 @@
         <v>1.9706496055853336E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B22" s="30"/>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B22" s="55" t="s">
+        <v>8</v>
+      </c>
       <c r="C22" s="25"/>
       <c r="D22" s="26"/>
       <c r="E22" s="31"/>
@@ -11820,7 +11828,7 @@
       <c r="R22" s="29"/>
       <c r="S22" s="34"/>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B23" s="47" t="s">
         <v>8</v>
       </c>
@@ -11892,7 +11900,7 @@
         <v>4.4643017846348901E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B24" s="47"/>
       <c r="C24" s="4" t="s">
         <v>18</v>
@@ -11962,7 +11970,7 @@
         <v>3.997170768273773E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B25" s="47"/>
       <c r="C25" s="4" t="s">
         <v>3</v>
@@ -12032,7 +12040,7 @@
         <v>4.987208440938274E-2</v>
       </c>
     </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B26" s="47"/>
       <c r="C26" s="4" t="s">
         <v>19</v>
@@ -12102,7 +12110,7 @@
         <v>3.8326001109827292E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B27" s="47"/>
       <c r="C27" s="4" t="s">
         <v>17</v>
@@ -12172,7 +12180,7 @@
         <v>3.6077666375167086E-2</v>
       </c>
     </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B28" s="47"/>
       <c r="C28" s="4" t="s">
         <v>4</v>
@@ -12242,7 +12250,7 @@
         <v>3.9652799941969304E-2</v>
       </c>
     </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B29" s="47"/>
       <c r="C29" s="4" t="s">
         <v>5</v>
@@ -12312,7 +12320,7 @@
         <v>4.4563019353375137E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B30" s="48"/>
       <c r="C30" s="4" t="s">
         <v>20</v>
@@ -12382,8 +12390,10 @@
         <v>4.853500899210151E-2</v>
       </c>
     </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B31" s="30"/>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B31" s="55" t="s">
+        <v>23</v>
+      </c>
       <c r="C31" s="25"/>
       <c r="D31" s="26"/>
       <c r="E31" s="31"/>
@@ -12402,7 +12412,7 @@
       <c r="R31" s="29"/>
       <c r="S31" s="34"/>
     </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B32" s="47" t="s">
         <v>23</v>
       </c>
@@ -12474,7 +12484,7 @@
         <v>4.0284146068368658E-2</v>
       </c>
     </row>
-    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B33" s="47"/>
       <c r="C33" s="4" t="s">
         <v>18</v>
@@ -12544,7 +12554,7 @@
         <v>3.621632839362391E-2</v>
       </c>
     </row>
-    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B34" s="47"/>
       <c r="C34" s="4" t="s">
         <v>3</v>
@@ -12614,7 +12624,7 @@
         <v>5.0893245309722293E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B35" s="47"/>
       <c r="C35" s="4" t="s">
         <v>19</v>
@@ -12684,7 +12694,7 @@
         <v>1.3929774849661306E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B36" s="47"/>
       <c r="C36" s="4" t="s">
         <v>17</v>
@@ -12754,7 +12764,7 @@
         <v>1.9587671820538728E-2</v>
       </c>
     </row>
-    <row r="37" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B37" s="47"/>
       <c r="C37" s="4" t="s">
         <v>4</v>
@@ -12824,7 +12834,7 @@
         <v>2.7874808831604404E-2</v>
       </c>
     </row>
-    <row r="38" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B38" s="47"/>
       <c r="C38" s="4" t="s">
         <v>5</v>
@@ -12894,7 +12904,7 @@
         <v>2.6347147377501812E-2</v>
       </c>
     </row>
-    <row r="39" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B39" s="48"/>
       <c r="C39" s="6" t="s">
         <v>20</v>
@@ -12973,8 +12983,44 @@
     <mergeCell ref="B14:B21"/>
     <mergeCell ref="B23:B30"/>
   </mergeCells>
+  <conditionalFormatting sqref="D5 F5 H5 J5 L5 N5 P5 R5">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7 F7 H7 J7 L7 N7 P7 R7">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D8 F8 H8 J8 L8 N8 P8 R8">
     <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9 F9 H9 J9 L9 N9 P9 R9">
+    <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -13057,186 +13103,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D23 F23 H23 J23 L23 N23 P23 R23">
-    <cfRule type="colorScale" priority="24">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F26 D26 H26 J26 L26 N26 P26 R26">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F27 D27 H27 J27 L27 N27 P27 R27">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D28 F28 H28 J28 L28 N28 P28 R28">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D29:D30 F29:F30 H29:H30 J29:J30 L29:L30 N29:N30 P29:P30 R29:R30">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F32 D32 H32 J32 L32 N32 P32 R32">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D33 F33 H33 J33 L33 N33 P33 R33">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D34 F34 H34 J34 L34 N34 P34 R34">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F35 D35 H35 J35 L35 N35 P35 R35">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F36 D36 H36 J36 L36 N36 P36 R36">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5 F5 H5 J5 L5 N5 P5 R5">
-    <cfRule type="colorScale" priority="40">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F6 D6 H6 J6 L6 N6 P6 R6">
-    <cfRule type="colorScale" priority="39">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7 F7 H7 J7 L7 N7 P7 R7">
-    <cfRule type="colorScale" priority="38">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D9 F9 H9 J9 L9 N9 P9 R9">
-    <cfRule type="colorScale" priority="36">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F11 D11 H11 J11 L11 N11 P11 R11">
-    <cfRule type="colorScale" priority="34">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D18 F18 H18 J18 L18 N18 P18 R18">
     <cfRule type="colorScale" priority="28">
       <colorScale>
@@ -13273,8 +13139,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21 D21 H21 J21 L21 N21 P21 R21">
-    <cfRule type="colorScale" priority="25">
+  <conditionalFormatting sqref="D23 F23 H23 J23 L23 N23 P23 R23">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -13297,6 +13163,102 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D28 F28 H28 J28 L28 N28 P28 R28">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29:D30 F29:F30 H29:H30 J29:J30 L29:L30 N29:N30 P29:P30 R29:R30">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33 F33 H33 J33 L33 N33 P33 R33">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34 F34 H34 J34 L34 N34 P34 R34">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37 F37 H37 J37 L37 N37 P37 R37">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6 D6 H6 J6 L6 N6 P6 R6">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11 D11 H11 J11 L11 N11 P11 R11">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21 D21 H21 J21 L21 N21 P21 R21">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F25 D25 H25 J25 L25 N25 P25 R25">
     <cfRule type="colorScale" priority="22">
       <colorScale>
@@ -13309,8 +13271,56 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37 F37 H37 J37 L37 N37 P37 R37">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="F26 D26 H26 J26 L26 N26 P26 R26">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F27 D27 H27 J27 L27 N27 P27 R27">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F32 D32 H32 J32 L32 N32 P32 R32">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F35 D35 H35 J35 L35 N35 P35 R35">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F36 D36 H36 J36 L36 N36 P36 R36">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -13355,22 +13365,22 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="11" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="16" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" style="16" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" style="16" customWidth="1"/>
-    <col min="20" max="20" width="1.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="11" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" style="16" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" customWidth="1"/>
+    <col min="16" max="16" width="10.6640625" style="16" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" style="16" customWidth="1"/>
+    <col min="20" max="20" width="1.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:25" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:25" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="str">
         <f>IF(Wind_overview_classifier!B2=0,"",Wind_overview_classifier!B2)</f>
         <v/>
@@ -13452,7 +13462,7 @@
       </c>
       <c r="Y2" s="54"/>
     </row>
-    <row r="3" spans="2:25" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:25" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="35" t="str">
         <f>IF(Wind_overview_classifier!B3=0,"",Wind_overview_classifier!B3)</f>
         <v>Model</v>
@@ -13526,10 +13536,10 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B4" s="24" t="str">
         <f>IF(Wind_overview_classifier!B4=0,"",Wind_overview_classifier!B4)</f>
-        <v/>
+        <v>ESC10</v>
       </c>
       <c r="C4" s="25" t="str">
         <f>IF(Wind_overview_classifier!C4=0,"",Wind_overview_classifier!C4)</f>
@@ -13600,7 +13610,7 @@
         <v>Std</v>
       </c>
     </row>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B5" s="53" t="str">
         <f>IF(Wind_overview_classifier!B5=0,"",Wind_overview_classifier!B5)</f>
         <v>ESC10</v>
@@ -13690,7 +13700,7 @@
         <v>-2.9738562091503495E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B6" s="47" t="str">
         <f>IF(Aug_overview_classifier!B6=0,"",Aug_overview_classifier!B6)</f>
         <v/>
@@ -13780,7 +13790,7 @@
         <v>-0.18308641975308693</v>
       </c>
     </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B7" s="47" t="str">
         <f>IF(Aug_overview_classifier!B7=0,"",Aug_overview_classifier!B7)</f>
         <v/>
@@ -13870,7 +13880,7 @@
         <v>-6.6782810685250382E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B8" s="47" t="str">
         <f>IF(Aug_overview_classifier!B8=0,"",Aug_overview_classifier!B8)</f>
         <v/>
@@ -13960,7 +13970,7 @@
         <v>-6.2133775566611704E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B9" s="47" t="str">
         <f>IF(Aug_overview_classifier!B9=0,"",Aug_overview_classifier!B9)</f>
         <v/>
@@ -14050,7 +14060,7 @@
         <v>-8.1578663211316793E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B10" s="47" t="str">
         <f>IF(Aug_overview_classifier!B10=0,"",Aug_overview_classifier!B10)</f>
         <v/>
@@ -14140,7 +14150,7 @@
         <v>-6.8330649490070283E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B11" s="47" t="str">
         <f>IF(Aug_overview_classifier!B11=0,"",Aug_overview_classifier!B11)</f>
         <v/>
@@ -14230,7 +14240,7 @@
         <v>-2.599286033021031E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B12" s="48" t="str">
         <f>IF(Aug_overview_classifier!B12=0,"",Aug_overview_classifier!B12)</f>
         <v/>
@@ -14320,10 +14330,10 @@
         <v>-1.3618233618233999E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B13" s="30" t="str">
         <f>IF(Wind_overview_classifier!B13=0,"",Wind_overview_classifier!B13)</f>
-        <v/>
+        <v>BDLib2</v>
       </c>
       <c r="C13" s="25" t="str">
         <f>IF(Wind_overview_classifier!C13=0,"",Wind_overview_classifier!C13)</f>
@@ -14404,7 +14414,7 @@
       </c>
       <c r="Y13" s="52"/>
     </row>
-    <row r="14" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B14" s="53" t="str">
         <f>IF(Wind_overview_classifier!B14=0,"",Wind_overview_classifier!B14)</f>
         <v>BDLib2</v>
@@ -14494,7 +14504,7 @@
         <v>-6.6764132553606692E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B15" s="47" t="str">
         <f>IF(Aug_overview_classifier!B15=0,"",Aug_overview_classifier!B15)</f>
         <v/>
@@ -14584,7 +14594,7 @@
         <v>-0.19017543859649166</v>
       </c>
     </row>
-    <row r="16" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B16" s="47" t="str">
         <f>IF(Aug_overview_classifier!B16=0,"",Aug_overview_classifier!B16)</f>
         <v/>
@@ -14674,7 +14684,7 @@
         <v>2.0520050125313549E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B17" s="47" t="str">
         <f>IF(Aug_overview_classifier!B17=0,"",Aug_overview_classifier!B17)</f>
         <v/>
@@ -14764,7 +14774,7 @@
         <v>-5.7268170426065579E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B18" s="47" t="str">
         <f>IF(Aug_overview_classifier!B18=0,"",Aug_overview_classifier!B18)</f>
         <v/>
@@ -14854,7 +14864,7 @@
         <v>1.5587044534412842E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B19" s="47" t="str">
         <f>IF(Aug_overview_classifier!B19=0,"",Aug_overview_classifier!B19)</f>
         <v/>
@@ -14944,7 +14954,7 @@
         <v>-2.1577666794723949E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B20" s="47" t="str">
         <f>IF(Aug_overview_classifier!B20=0,"",Aug_overview_classifier!B20)</f>
         <v/>
@@ -15034,7 +15044,7 @@
         <v>0.11820534943917083</v>
       </c>
     </row>
-    <row r="21" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B21" s="48" t="str">
         <f>IF(Aug_overview_classifier!B21=0,"",Aug_overview_classifier!B21)</f>
         <v/>
@@ -15124,10 +15134,10 @@
         <v>0.19658521303258114</v>
       </c>
     </row>
-    <row r="22" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B22" s="30" t="str">
         <f>IF(Wind_overview_classifier!B22=0,"",Wind_overview_classifier!B22)</f>
-        <v/>
+        <v>US8K</v>
       </c>
       <c r="C22" s="25" t="str">
         <f>IF(Wind_overview_classifier!C22=0,"",Wind_overview_classifier!C22)</f>
@@ -15208,7 +15218,7 @@
       </c>
       <c r="Y22" s="52"/>
     </row>
-    <row r="23" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B23" s="53" t="str">
         <f>IF(Wind_overview_classifier!B23=0,"",Wind_overview_classifier!B23)</f>
         <v>US8K</v>
@@ -15298,7 +15308,7 @@
         <v>-7.3305794695187276E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B24" s="47" t="str">
         <f>IF(Aug_overview_classifier!B24=0,"",Aug_overview_classifier!B24)</f>
         <v/>
@@ -15388,7 +15398,7 @@
         <v>-0.19428799285871357</v>
       </c>
     </row>
-    <row r="25" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B25" s="47" t="str">
         <f>IF(Aug_overview_classifier!B25=0,"",Aug_overview_classifier!B25)</f>
         <v/>
@@ -15478,7 +15488,7 @@
         <v>-6.8259235188211864E-2</v>
       </c>
     </row>
-    <row r="26" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B26" s="47" t="str">
         <f>IF(Aug_overview_classifier!B26=0,"",Aug_overview_classifier!B26)</f>
         <v/>
@@ -15568,7 +15578,7 @@
         <v>-5.7821717769824699E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B27" s="47" t="str">
         <f>IF(Aug_overview_classifier!B27=0,"",Aug_overview_classifier!B27)</f>
         <v/>
@@ -15658,7 +15668,7 @@
         <v>-3.1772301279066273E-2</v>
       </c>
     </row>
-    <row r="28" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B28" s="47" t="str">
         <f>IF(Aug_overview_classifier!B28=0,"",Aug_overview_classifier!B28)</f>
         <v/>
@@ -15748,7 +15758,7 @@
         <v>-3.9738486748595259E-2</v>
       </c>
     </row>
-    <row r="29" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B29" s="47" t="str">
         <f>IF(Aug_overview_classifier!B29=0,"",Aug_overview_classifier!B29)</f>
         <v/>
@@ -15838,7 +15848,7 @@
         <v>-7.1847142469436576E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B30" s="48" t="str">
         <f>IF(Aug_overview_classifier!B30=0,"",Aug_overview_classifier!B30)</f>
         <v/>
@@ -15928,10 +15938,10 @@
         <v>-0.11535844087849767</v>
       </c>
     </row>
-    <row r="31" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B31" s="30" t="str">
         <f>IF(Wind_overview_classifier!B31=0,"",Wind_overview_classifier!B31)</f>
-        <v/>
+        <v>US8K_AV</v>
       </c>
       <c r="C31" s="25" t="str">
         <f>IF(Wind_overview_classifier!C31=0,"",Wind_overview_classifier!C31)</f>
@@ -16012,7 +16022,7 @@
       </c>
       <c r="Y31" s="52"/>
     </row>
-    <row r="32" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B32" s="53" t="str">
         <f>IF(Wind_overview_classifier!B32=0,"",Wind_overview_classifier!B32)</f>
         <v>US8K_AV</v>
@@ -16102,7 +16112,7 @@
         <v>-5.2915939256235056E-2</v>
       </c>
     </row>
-    <row r="33" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B33" s="47" t="str">
         <f>IF(Aug_overview_classifier!B33=0,"",Aug_overview_classifier!B33)</f>
         <v/>
@@ -16192,7 +16202,7 @@
         <v>-6.2138101270161172E-2</v>
       </c>
     </row>
-    <row r="34" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B34" s="47" t="str">
         <f>IF(Aug_overview_classifier!B34=0,"",Aug_overview_classifier!B34)</f>
         <v/>
@@ -16282,7 +16292,7 @@
         <v>-4.9160061745109562E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B35" s="47" t="str">
         <f>IF(Aug_overview_classifier!B35=0,"",Aug_overview_classifier!B35)</f>
         <v/>
@@ -16372,7 +16382,7 @@
         <v>-5.4365459411869876E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B36" s="47" t="str">
         <f>IF(Aug_overview_classifier!B36=0,"",Aug_overview_classifier!B36)</f>
         <v/>
@@ -16462,7 +16472,7 @@
         <v>-3.9384666074033903E-2</v>
       </c>
     </row>
-    <row r="37" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B37" s="47" t="str">
         <f>IF(Aug_overview_classifier!B37=0,"",Aug_overview_classifier!B37)</f>
         <v/>
@@ -16552,7 +16562,7 @@
         <v>-3.7631188310879193E-2</v>
       </c>
     </row>
-    <row r="38" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B38" s="47" t="str">
         <f>IF(Aug_overview_classifier!B38=0,"",Aug_overview_classifier!B38)</f>
         <v/>
@@ -16642,7 +16652,7 @@
         <v>-7.3449125638510915E-2</v>
       </c>
     </row>
-    <row r="39" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B39" s="48" t="str">
         <f>IF(Aug_overview_classifier!B39=0,"",Aug_overview_classifier!B39)</f>
         <v/>
@@ -16732,7 +16742,7 @@
         <v>-4.8129389550780499E-2</v>
       </c>
     </row>
-    <row r="40" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:25" x14ac:dyDescent="0.3">
       <c r="U40" s="52">
         <f>AVERAGE(U32:V39)</f>
         <v>-4.4885044745957267E-2</v>
@@ -16843,22 +16853,4 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EB4F2EF-885C-4022-AB47-D5989E6E71D1}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Adjustments based on the last tests
</commit_message>
<xml_diff>
--- a/_analysis/_Results_compilation_training_flow_2024_06.xlsx
+++ b/_analysis/_Results_compilation_training_flow_2024_06.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Andre_Florentino\03_particular\04_mestrado-FEI\97_master\_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2DA3A8-68C6-4645-8329-E35ACA33D405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA682AD4-4923-4394-857D-8FF02E1B1188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{765D2107-F650-4F10-ACE3-9E968F4DE976}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{765D2107-F650-4F10-ACE3-9E968F4DE976}"/>
   </bookViews>
   <sheets>
     <sheet name="Aug_overview_classifier" sheetId="1" r:id="rId1"/>
@@ -567,6 +567,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -595,9 +598,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4477,63 +4477,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C84E9B-02A8-4A6E-9A9C-4104E745268F}">
   <dimension ref="B2:S39"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="11" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" style="16" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" customWidth="1"/>
-    <col min="16" max="16" width="10.6640625" style="16" customWidth="1"/>
-    <col min="18" max="18" width="10.6640625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="11" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="16" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" style="16" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:19" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="12"/>
       <c r="C2" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="45" t="s">
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="46" t="s">
+      <c r="M2" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="46" t="s">
+      <c r="N2" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="46" t="s">
+      <c r="O2" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="P2" s="46" t="s">
+      <c r="P2" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="Q2" s="46" t="s">
+      <c r="Q2" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="R2" s="46" t="s">
+      <c r="R2" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="46" t="s">
+      <c r="S2" s="47" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="2:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="35" t="s">
         <v>15</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="24"/>
       <c r="C4" s="25"/>
       <c r="D4" s="26" t="s">
@@ -4631,8 +4631,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B5" s="47" t="s">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="48" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -4703,8 +4703,8 @@
         <v>2.7099354235848503E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B6" s="47"/>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B6" s="48"/>
       <c r="C6" s="4" t="s">
         <v>18</v>
       </c>
@@ -4773,8 +4773,8 @@
         <v>8.0719421454814852E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B7" s="47"/>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="48"/>
       <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
@@ -4843,8 +4843,8 @@
         <v>5.7008771254956896E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B8" s="47"/>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="48"/>
       <c r="C8" s="4" t="s">
         <v>19</v>
       </c>
@@ -4913,8 +4913,8 @@
         <v>5.659615711335883E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B9" s="47"/>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="48"/>
       <c r="C9" s="4" t="s">
         <v>17</v>
       </c>
@@ -4983,8 +4983,8 @@
         <v>7.725768570181224E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B10" s="47"/>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B10" s="48"/>
       <c r="C10" s="4" t="s">
         <v>4</v>
       </c>
@@ -5053,8 +5053,8 @@
         <v>4.5586456322026181E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B11" s="47"/>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B11" s="48"/>
       <c r="C11" s="4" t="s">
         <v>5</v>
       </c>
@@ -5123,8 +5123,8 @@
         <v>4.183300132670377E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B12" s="48"/>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B12" s="49"/>
       <c r="C12" s="6" t="s">
         <v>20</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>4.6770717334674264E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B13" s="30"/>
       <c r="C13" s="25"/>
       <c r="D13" s="26"/>
@@ -5213,8 +5213,8 @@
       <c r="R13" s="29"/>
       <c r="S13" s="34"/>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B14" s="47" t="s">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B14" s="48" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -5285,8 +5285,8 @@
         <v>5.3575837561071885E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B15" s="47"/>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B15" s="48"/>
       <c r="C15" s="4" t="s">
         <v>18</v>
       </c>
@@ -5355,8 +5355,8 @@
         <v>9.6225044864939862E-3</v>
       </c>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B16" s="47"/>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B16" s="48"/>
       <c r="C16" s="4" t="s">
         <v>3</v>
       </c>
@@ -5425,8 +5425,8 @@
         <v>2.5458753860865761E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B17" s="47"/>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B17" s="48"/>
       <c r="C17" s="4" t="s">
         <v>19</v>
       </c>
@@ -5495,8 +5495,8 @@
         <v>6.3098981620002811E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B18" s="47"/>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B18" s="48"/>
       <c r="C18" s="4" t="s">
         <v>17</v>
       </c>
@@ -5565,8 +5565,8 @@
         <v>1.9245008972987331E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B19" s="47"/>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B19" s="48"/>
       <c r="C19" s="4" t="s">
         <v>4</v>
       </c>
@@ -5635,8 +5635,8 @@
         <v>5.3575837561072148E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B20" s="47"/>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B20" s="48"/>
       <c r="C20" s="4" t="s">
         <v>5</v>
       </c>
@@ -5705,8 +5705,8 @@
         <v>3.4694433324435663E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B21" s="48"/>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B21" s="49"/>
       <c r="C21" s="6" t="s">
         <v>20</v>
       </c>
@@ -5775,7 +5775,7 @@
         <v>1.6666666666666496E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B22" s="30"/>
       <c r="C22" s="25"/>
       <c r="D22" s="26"/>
@@ -5795,8 +5795,8 @@
       <c r="R22" s="29"/>
       <c r="S22" s="34"/>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B23" s="47" t="s">
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B23" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -5867,8 +5867,8 @@
         <v>4.4362319217983379E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B24" s="47"/>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B24" s="48"/>
       <c r="C24" s="4" t="s">
         <v>18</v>
       </c>
@@ -5937,8 +5937,8 @@
         <v>5.0363616429460974E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B25" s="47"/>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B25" s="48"/>
       <c r="C25" s="4" t="s">
         <v>3</v>
       </c>
@@ -6007,8 +6007,8 @@
         <v>6.1554295024420218E-2</v>
       </c>
     </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B26" s="47"/>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B26" s="48"/>
       <c r="C26" s="4" t="s">
         <v>19</v>
       </c>
@@ -6077,8 +6077,8 @@
         <v>2.962107369301108E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B27" s="47"/>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B27" s="48"/>
       <c r="C27" s="4" t="s">
         <v>17</v>
       </c>
@@ -6147,8 +6147,8 @@
         <v>3.1220495989087861E-2</v>
       </c>
     </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B28" s="47"/>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B28" s="48"/>
       <c r="C28" s="4" t="s">
         <v>4</v>
       </c>
@@ -6217,8 +6217,8 @@
         <v>3.5253353024031292E-2</v>
       </c>
     </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B29" s="47"/>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B29" s="48"/>
       <c r="C29" s="4" t="s">
         <v>5</v>
       </c>
@@ -6287,8 +6287,8 @@
         <v>4.1853247574758473E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B30" s="48"/>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B30" s="49"/>
       <c r="C30" s="6" t="s">
         <v>20</v>
       </c>
@@ -6357,7 +6357,7 @@
         <v>4.2097691385037841E-2</v>
       </c>
     </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B31" s="30"/>
       <c r="C31" s="25"/>
       <c r="D31" s="26"/>
@@ -6377,8 +6377,8 @@
       <c r="R31" s="29"/>
       <c r="S31" s="34"/>
     </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B32" s="47" t="s">
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B32" s="48" t="s">
         <v>23</v>
       </c>
       <c r="C32" s="2" t="s">
@@ -6449,8 +6449,8 @@
         <v>5.2680761025622622E-2</v>
       </c>
     </row>
-    <row r="33" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B33" s="47"/>
+    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B33" s="48"/>
       <c r="C33" s="4" t="s">
         <v>18</v>
       </c>
@@ -6519,8 +6519,8 @@
         <v>4.8661670511817759E-2</v>
       </c>
     </row>
-    <row r="34" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B34" s="47"/>
+    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B34" s="48"/>
       <c r="C34" s="4" t="s">
         <v>3</v>
       </c>
@@ -6589,8 +6589,8 @@
         <v>4.6344311238478736E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B35" s="47"/>
+    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B35" s="48"/>
       <c r="C35" s="4" t="s">
         <v>19</v>
       </c>
@@ -6659,8 +6659,8 @@
         <v>2.4772141992337307E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B36" s="47"/>
+    <row r="36" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B36" s="48"/>
       <c r="C36" s="4" t="s">
         <v>17</v>
       </c>
@@ -6729,8 +6729,8 @@
         <v>2.3219868574884551E-2</v>
       </c>
     </row>
-    <row r="37" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B37" s="47"/>
+    <row r="37" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B37" s="48"/>
       <c r="C37" s="4" t="s">
         <v>4</v>
       </c>
@@ -6799,8 +6799,8 @@
         <v>3.405096917308921E-2</v>
       </c>
     </row>
-    <row r="38" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B38" s="47"/>
+    <row r="38" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B38" s="48"/>
       <c r="C38" s="4" t="s">
         <v>5</v>
       </c>
@@ -6869,8 +6869,8 @@
         <v>2.9455118821827914E-2</v>
       </c>
     </row>
-    <row r="39" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B39" s="48"/>
+    <row r="39" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B39" s="49"/>
       <c r="C39" s="6" t="s">
         <v>20</v>
       </c>
@@ -6948,7 +6948,307 @@
     <mergeCell ref="B23:B30"/>
     <mergeCell ref="D2:K2"/>
   </mergeCells>
-  <conditionalFormatting sqref="D6 F6 H6 J6 L6 N6 P6 R6">
+  <conditionalFormatting sqref="D5 F5 H5 J5 L5 N5 P5 R5">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8 F8 H8 J8 L8 N8 P8 R8">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9 F9 H9 J9 L9 N9 P9 R9">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11 F11 H11 J11 L11 N11 P11 R11">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12 F12 H12 J12 L12 N12 P12 R12">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16 F16 H16 J16 L16 N16 P16 R16">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17 F17 H17 J17 L17 N17 P17 R17">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18 F18 H18 J18 L18 N18 P18 R18">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19 F19 H19 J19 L19 N19 P19 R19">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20 F20 H20 J20 L20 N20 P20 R20">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21 F21 H21 J21 L21 N21 P21 R21">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23 F23 H23 J23 L23 N23 P23 R23">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24 F24 H24 J24 L24 N24 P24 R24">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25 F25 H25 J25 L25 N25 P25 R25">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26 F26 H26 J26 L26 N26 P26 R26">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27 F27 H27 J27 L27 N27 P27 R27">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28 F28 H28 J28 L28 N28 P28 R28">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30 F30 H30 J30 L30 N30 P30 R30">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33 F33 H33 J33 L33 N33 P33 R33">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34 F34 H34 J34 L34 N34 P34 R34">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35 F35 H35 J35 L35 N35 P35 R35">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36 F36 H36 J36 L36 N36 P36 R36">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37 F37 H37 J37 L37 N37 P37 R37">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38 F38 H38 J38 L38 N38 P38 R38">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39 F39 H39 J39 L39 N39 P39 R39">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6 D6 H6 J6 L6 N6 P6 R6">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
@@ -6960,7 +7260,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7 F7 H7 J7 L7 N7 P7 R7">
+  <conditionalFormatting sqref="F7 D7 H7 J7 L7 N7 P7 R7">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
@@ -6972,7 +7272,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10 F10 H10 J10 L10 N10 P10 R10">
+  <conditionalFormatting sqref="F10 D10 H10 J10 L10 N10 P10 R10">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -6984,7 +7284,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14 F14 H14 J14 L14 N14 P14 R14">
+  <conditionalFormatting sqref="F14 D14 H14 J14 L14 N14 P14 R14">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -6996,7 +7296,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15 F15 H15 J15 L15 N15 P15 R15">
+  <conditionalFormatting sqref="F15 D15 H15 J15 L15 N15 P15 R15">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -7008,7 +7308,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D29 F29 H29 J29 L29 N29 P29 R29">
+  <conditionalFormatting sqref="F29 D29 H29 J29 L29 N29 P29 R29">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -7020,308 +7320,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32 F32 H32 J32 L32 N32 P32 R32">
+  <conditionalFormatting sqref="F32 D32 H32 J32 L32 N32 P32 R32">
     <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5 D5 H5 J5 L5 N5 P5 R5">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8 D8 H8 J8 L8 N8 P8 R8">
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F9 D9 H9 J9 L9 N9 P9 R9">
-    <cfRule type="colorScale" priority="28">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F11 D11 H11 J11 L11 N11 P11 R11">
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12 D12 H12 J12 L12 N12 P12 R12">
-    <cfRule type="colorScale" priority="25">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F16 D16 H16 J16 L16 N16 P16 R16">
-    <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F17 D17 H17 J17 L17 N17 P17 R17">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F18 D18 H18 J18 L18 N18 P18 R18">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F19 D19 H19 J19 L19 N19 P19 R19">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F20 D20 H20 J20 L20 N20 P20 R20">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F21 D21 H21 J21 L21 N21 P21 R21">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F23 D23 H23 J23 L23 N23 P23 R23">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F24 D24 H24 J24 L24 N24 P24 R24">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F25 D25 H25 J25 L25 N25 P25 R25">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F26 D26 H26 J26 L26 N26 P26 R26">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F27 D27 H27 J27 L27 N27 P27 R27">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F28 D28 H28 J28 L28 N28 P28 R28">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F30 D30 H30 J30 L30 N30 P30 R30">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F33 D33 H33 J33 L33 N33 P33 R33">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F34 D34 H34 J34 L34 N34 P34 R34">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F35 D35 H35 J35 L35 N35 P35 R35">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F36 D36 H36 J36 L36 N36 P36 R36">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F37 D37 H37 J37 L37 N37 P37 R37">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F38 D38 H38 J38 L38 N38 P38 R38">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F39 D39 H39 J39 L39 N39 P39 R39">
-    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7342,22 +7342,22 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="11" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" style="16" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" customWidth="1"/>
-    <col min="16" max="16" width="10.6640625" style="16" customWidth="1"/>
-    <col min="18" max="18" width="10.6640625" style="16" customWidth="1"/>
-    <col min="20" max="20" width="1.6640625" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="11" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="16" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" style="16" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" style="16" customWidth="1"/>
+    <col min="20" max="20" width="1.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:22" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:22" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="12" t="str">
         <f>IF(Aug_overview_classifier!B2=0,"",Aug_overview_classifier!B2)</f>
         <v/>
@@ -7366,72 +7366,72 @@
         <f>IF(Aug_overview_classifier!C2=0,"",Aug_overview_classifier!C2)</f>
         <v>Classifiers</v>
       </c>
-      <c r="D2" s="49" t="str">
+      <c r="D2" s="50" t="str">
         <f>IF(Aug_overview_classifier!D2=0,"",Aug_overview_classifier!D2)</f>
         <v>Augmented</v>
       </c>
-      <c r="E2" s="50" t="str">
+      <c r="E2" s="51" t="str">
         <f>IF(Aug_overview_classifier!E2=0,"",Aug_overview_classifier!E2)</f>
         <v/>
       </c>
-      <c r="F2" s="50" t="str">
+      <c r="F2" s="51" t="str">
         <f>IF(Aug_overview_classifier!F2=0,"",Aug_overview_classifier!F2)</f>
         <v/>
       </c>
-      <c r="G2" s="50" t="str">
+      <c r="G2" s="51" t="str">
         <f>IF(Aug_overview_classifier!G2=0,"",Aug_overview_classifier!G2)</f>
         <v/>
       </c>
-      <c r="H2" s="50" t="str">
+      <c r="H2" s="51" t="str">
         <f>IF(Aug_overview_classifier!H2=0,"",Aug_overview_classifier!H2)</f>
         <v/>
       </c>
-      <c r="I2" s="50" t="str">
+      <c r="I2" s="51" t="str">
         <f>IF(Aug_overview_classifier!I2=0,"",Aug_overview_classifier!I2)</f>
         <v/>
       </c>
-      <c r="J2" s="50" t="str">
+      <c r="J2" s="51" t="str">
         <f>IF(Aug_overview_classifier!J2=0,"",Aug_overview_classifier!J2)</f>
         <v/>
       </c>
-      <c r="K2" s="51" t="str">
+      <c r="K2" s="52" t="str">
         <f>IF(Aug_overview_classifier!K2=0,"",Aug_overview_classifier!K2)</f>
         <v/>
       </c>
-      <c r="L2" s="45" t="str">
+      <c r="L2" s="46" t="str">
         <f>IF(Aug_overview_classifier!L2=0,"",Aug_overview_classifier!L2)</f>
         <v>Original</v>
       </c>
-      <c r="M2" s="46" t="str">
+      <c r="M2" s="47" t="str">
         <f>IF(Aug_overview_classifier!M2=0,"",Aug_overview_classifier!M2)</f>
         <v/>
       </c>
-      <c r="N2" s="46" t="str">
+      <c r="N2" s="47" t="str">
         <f>IF(Aug_overview_classifier!N2=0,"",Aug_overview_classifier!N2)</f>
         <v/>
       </c>
-      <c r="O2" s="46" t="str">
+      <c r="O2" s="47" t="str">
         <f>IF(Aug_overview_classifier!O2=0,"",Aug_overview_classifier!O2)</f>
         <v/>
       </c>
-      <c r="P2" s="46" t="str">
+      <c r="P2" s="47" t="str">
         <f>IF(Aug_overview_classifier!P2=0,"",Aug_overview_classifier!P2)</f>
         <v/>
       </c>
-      <c r="Q2" s="46" t="str">
+      <c r="Q2" s="47" t="str">
         <f>IF(Aug_overview_classifier!Q2=0,"",Aug_overview_classifier!Q2)</f>
         <v/>
       </c>
-      <c r="R2" s="46" t="str">
+      <c r="R2" s="47" t="str">
         <f>IF(Aug_overview_classifier!R2=0,"",Aug_overview_classifier!R2)</f>
         <v/>
       </c>
-      <c r="S2" s="46" t="str">
+      <c r="S2" s="47" t="str">
         <f>IF(Aug_overview_classifier!S2=0,"",Aug_overview_classifier!S2)</f>
         <v/>
       </c>
     </row>
-    <row r="3" spans="2:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="35" t="str">
         <f>IF(Aug_overview_classifier!B3=0,"",Aug_overview_classifier!B3)</f>
         <v>Model</v>
@@ -7505,7 +7505,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="24" t="str">
         <f>IF(Aug_overview_classifier!B4=0,"",Aug_overview_classifier!B4)</f>
         <v/>
@@ -7579,8 +7579,8 @@
         <v>Std</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B5" s="53" t="str">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B5" s="54" t="str">
         <f>IF(Aug_overview_classifier!B5=0,"",Aug_overview_classifier!B5)</f>
         <v>ESC10</v>
       </c>
@@ -7661,8 +7661,8 @@
         <v>2.3529411764705577E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B6" s="47" t="str">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B6" s="48" t="str">
         <f>IF(Aug_overview_classifier!B6=0,"",Aug_overview_classifier!B6)</f>
         <v/>
       </c>
@@ -7743,8 +7743,8 @@
         <v>-2.8333333333333655E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B7" s="47" t="str">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B7" s="48" t="str">
         <f>IF(Aug_overview_classifier!B7=0,"",Aug_overview_classifier!B7)</f>
         <v/>
       </c>
@@ -7825,8 +7825,8 @@
         <v>2.7874564459930085E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B8" s="47" t="str">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="48" t="str">
         <f>IF(Aug_overview_classifier!B8=0,"",Aug_overview_classifier!B8)</f>
         <v/>
       </c>
@@ -7907,8 +7907,8 @@
         <v>1.293532338308423E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B9" s="47" t="str">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="48" t="str">
         <f>IF(Aug_overview_classifier!B9=0,"",Aug_overview_classifier!B9)</f>
         <v/>
       </c>
@@ -7989,8 +7989,8 @@
         <v>-2.9154518950438302E-3</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B10" s="47" t="str">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="48" t="str">
         <f>IF(Aug_overview_classifier!B10=0,"",Aug_overview_classifier!B10)</f>
         <v/>
       </c>
@@ -8071,8 +8071,8 @@
         <v>5.3140096618353727E-3</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B11" s="47" t="str">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B11" s="48" t="str">
         <f>IF(Aug_overview_classifier!B11=0,"",Aug_overview_classifier!B11)</f>
         <v/>
       </c>
@@ -8153,8 +8153,8 @@
         <v>3.2630522088352931E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B12" s="48" t="str">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B12" s="49" t="str">
         <f>IF(Aug_overview_classifier!B12=0,"",Aug_overview_classifier!B12)</f>
         <v/>
       </c>
@@ -8235,7 +8235,7 @@
         <v>4.5641025641025346E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B13" s="30" t="str">
         <f>IF(Aug_overview_classifier!B13=0,"",Aug_overview_classifier!B13)</f>
         <v/>
@@ -8308,14 +8308,14 @@
         <f>IF(Aug_overview_classifier!S13=0,"",Aug_overview_classifier!S13)</f>
         <v/>
       </c>
-      <c r="U13" s="52">
+      <c r="U13" s="53">
         <f>AVERAGE(U5:V12)</f>
         <v>9.931847414804941E-3</v>
       </c>
-      <c r="V13" s="52"/>
+      <c r="V13" s="53"/>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B14" s="53" t="str">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="54" t="str">
         <f>IF(Aug_overview_classifier!B14=0,"",Aug_overview_classifier!B14)</f>
         <v>BDLib2</v>
       </c>
@@ -8396,8 +8396,8 @@
         <v>-5.7870370370370905E-3</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B15" s="47" t="str">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="48" t="str">
         <f>IF(Aug_overview_classifier!B15=0,"",Aug_overview_classifier!B15)</f>
         <v/>
       </c>
@@ -8478,8 +8478,8 @@
         <v>-4.4000000000000372E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B16" s="47" t="str">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B16" s="48" t="str">
         <f>IF(Aug_overview_classifier!B16=0,"",Aug_overview_classifier!B16)</f>
         <v/>
       </c>
@@ -8560,8 +8560,8 @@
         <v>6.8452380952381153E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B17" s="47" t="str">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B17" s="48" t="str">
         <f>IF(Aug_overview_classifier!B17=0,"",Aug_overview_classifier!B17)</f>
         <v/>
       </c>
@@ -8642,8 +8642,8 @@
         <v>9.5238095238090459E-3</v>
       </c>
     </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B18" s="47" t="str">
+    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B18" s="48" t="str">
         <f>IF(Aug_overview_classifier!B18=0,"",Aug_overview_classifier!B18)</f>
         <v/>
       </c>
@@ -8724,8 +8724,8 @@
         <v>7.051282051282004E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B19" s="47" t="str">
+    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B19" s="48" t="str">
         <f>IF(Aug_overview_classifier!B19=0,"",Aug_overview_classifier!B19)</f>
         <v/>
       </c>
@@ -8806,8 +8806,8 @@
         <v>2.3114355231143913E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B20" s="47" t="str">
+    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B20" s="48" t="str">
         <f>IF(Aug_overview_classifier!B20=0,"",Aug_overview_classifier!B20)</f>
         <v/>
       </c>
@@ -8888,8 +8888,8 @@
         <v>0.17622950819672112</v>
       </c>
     </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B21" s="48" t="str">
+    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B21" s="49" t="str">
         <f>IF(Aug_overview_classifier!B21=0,"",Aug_overview_classifier!B21)</f>
         <v/>
       </c>
@@ -8970,7 +8970,7 @@
         <v>0.18303571428571397</v>
       </c>
     </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B22" s="30" t="str">
         <f>IF(Aug_overview_classifier!B22=0,"",Aug_overview_classifier!B22)</f>
         <v/>
@@ -9043,14 +9043,14 @@
         <f>IF(Aug_overview_classifier!S22=0,"",Aug_overview_classifier!S22)</f>
         <v/>
       </c>
-      <c r="U22" s="52">
+      <c r="U22" s="53">
         <f>AVERAGE(U14:V21)</f>
         <v>5.9056245465618183E-2</v>
       </c>
-      <c r="V22" s="52"/>
+      <c r="V22" s="53"/>
     </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B23" s="53" t="str">
+    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B23" s="54" t="str">
         <f>IF(Aug_overview_classifier!B23=0,"",Aug_overview_classifier!B23)</f>
         <v>US8K</v>
       </c>
@@ -9131,8 +9131,8 @@
         <v>-1.6213829198711283E-3</v>
       </c>
     </row>
-    <row r="24" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B24" s="47" t="str">
+    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B24" s="48" t="str">
         <f>IF(Aug_overview_classifier!B24=0,"",Aug_overview_classifier!B24)</f>
         <v/>
       </c>
@@ -9213,8 +9213,8 @@
         <v>-6.9708096779339646E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B25" s="47" t="str">
+    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B25" s="48" t="str">
         <f>IF(Aug_overview_classifier!B25=0,"",Aug_overview_classifier!B25)</f>
         <v/>
       </c>
@@ -9295,8 +9295,8 @@
         <v>1.4505669218352057E-2</v>
       </c>
     </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B26" s="47" t="str">
+    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B26" s="48" t="str">
         <f>IF(Aug_overview_classifier!B26=0,"",Aug_overview_classifier!B26)</f>
         <v/>
       </c>
@@ -9377,8 +9377,8 @@
         <v>-1.4666102087111943E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B27" s="47" t="str">
+    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B27" s="48" t="str">
         <f>IF(Aug_overview_classifier!B27=0,"",Aug_overview_classifier!B27)</f>
         <v/>
       </c>
@@ -9459,8 +9459,8 @@
         <v>1.4307751856672102E-2</v>
       </c>
     </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B28" s="47" t="str">
+    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B28" s="48" t="str">
         <f>IF(Aug_overview_classifier!B28=0,"",Aug_overview_classifier!B28)</f>
         <v/>
       </c>
@@ -9541,8 +9541,8 @@
         <v>-1.9345565361934547E-3</v>
       </c>
     </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B29" s="47" t="str">
+    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B29" s="48" t="str">
         <f>IF(Aug_overview_classifier!B29=0,"",Aug_overview_classifier!B29)</f>
         <v/>
       </c>
@@ -9623,8 +9623,8 @@
         <v>-1.714759822894385E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B30" s="48" t="str">
+    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B30" s="49" t="str">
         <f>IF(Aug_overview_classifier!B30=0,"",Aug_overview_classifier!B30)</f>
         <v/>
       </c>
@@ -9705,7 +9705,7 @@
         <v>-1.128752492413998E-2</v>
       </c>
     </row>
-    <row r="31" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B31" s="30" t="str">
         <f>IF(Aug_overview_classifier!B31=0,"",Aug_overview_classifier!B31)</f>
         <v/>
@@ -9778,14 +9778,14 @@
         <f>IF(Aug_overview_classifier!S31=0,"",Aug_overview_classifier!S31)</f>
         <v/>
       </c>
-      <c r="U31" s="52">
+      <c r="U31" s="53">
         <f>AVERAGE(U23:V30)</f>
         <v>-1.4491331682895237E-2</v>
       </c>
-      <c r="V31" s="52"/>
+      <c r="V31" s="53"/>
     </row>
-    <row r="32" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B32" s="53" t="str">
+    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B32" s="54" t="str">
         <f>IF(Aug_overview_classifier!B32=0,"",Aug_overview_classifier!B32)</f>
         <v>US8K_AV</v>
       </c>
@@ -9866,8 +9866,8 @@
         <v>-2.6953488532588388E-4</v>
       </c>
     </row>
-    <row r="33" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B33" s="47" t="str">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B33" s="48" t="str">
         <f>IF(Aug_overview_classifier!B33=0,"",Aug_overview_classifier!B33)</f>
         <v/>
       </c>
@@ -9948,8 +9948,8 @@
         <v>-6.5164732424990657E-2</v>
       </c>
     </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B34" s="47" t="str">
+    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B34" s="48" t="str">
         <f>IF(Aug_overview_classifier!B34=0,"",Aug_overview_classifier!B34)</f>
         <v/>
       </c>
@@ -10030,8 +10030,8 @@
         <v>1.2094980093515062E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B35" s="47" t="str">
+    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B35" s="48" t="str">
         <f>IF(Aug_overview_classifier!B35=0,"",Aug_overview_classifier!B35)</f>
         <v/>
       </c>
@@ -10112,8 +10112,8 @@
         <v>-1.6341243577944531E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B36" s="47" t="str">
+    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B36" s="48" t="str">
         <f>IF(Aug_overview_classifier!B36=0,"",Aug_overview_classifier!B36)</f>
         <v/>
       </c>
@@ -10194,8 +10194,8 @@
         <v>1.7515293515845798E-2</v>
       </c>
     </row>
-    <row r="37" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B37" s="47" t="str">
+    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B37" s="48" t="str">
         <f>IF(Aug_overview_classifier!B37=0,"",Aug_overview_classifier!B37)</f>
         <v/>
       </c>
@@ -10276,8 +10276,8 @@
         <v>-3.3792627557065469E-3</v>
       </c>
     </row>
-    <row r="38" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B38" s="47" t="str">
+    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B38" s="48" t="str">
         <f>IF(Aug_overview_classifier!B38=0,"",Aug_overview_classifier!B38)</f>
         <v/>
       </c>
@@ -10358,8 +10358,8 @@
         <v>-5.2653729105160973E-3</v>
       </c>
     </row>
-    <row r="39" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B39" s="48" t="str">
+    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B39" s="49" t="str">
         <f>IF(Aug_overview_classifier!B39=0,"",Aug_overview_classifier!B39)</f>
         <v/>
       </c>
@@ -10440,12 +10440,12 @@
         <v>1.3389813031775333E-2</v>
       </c>
     </row>
-    <row r="40" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="U40" s="52">
+    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="U40" s="53">
         <f>AVERAGE(U32:V39)</f>
         <v>-1.0565448561979364E-2</v>
       </c>
-      <c r="V40" s="52"/>
+      <c r="V40" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -10526,49 +10526,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5498D750-A77C-4E1F-AC8E-4A19415168F1}">
   <dimension ref="B2:S39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="11" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" style="16" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" customWidth="1"/>
-    <col min="16" max="16" width="10.6640625" style="16" customWidth="1"/>
-    <col min="18" max="18" width="10.6640625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="11" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="16" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" style="16" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:19" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="12"/>
       <c r="C2" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="45" t="s">
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
     </row>
-    <row r="3" spans="2:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="35" t="s">
         <v>15</v>
       </c>
@@ -10606,8 +10606,8 @@
       </c>
       <c r="S3" s="38"/>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B4" s="55" t="s">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B4" s="45" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="25"/>
@@ -10660,8 +10660,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="47" t="s">
+    <row r="5" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="48" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -10732,8 +10732,8 @@
         <v>3.6554510121453804E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="47"/>
+    <row r="6" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="48"/>
       <c r="C6" s="4" t="s">
         <v>18</v>
       </c>
@@ -10802,8 +10802,8 @@
         <v>4.3329907964490905E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="47"/>
+    <row r="7" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="48"/>
       <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
@@ -10872,8 +10872,8 @@
         <v>4.4837729927308778E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="47"/>
+    <row r="8" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="48"/>
       <c r="C8" s="4" t="s">
         <v>19</v>
       </c>
@@ -10942,8 +10942,8 @@
         <v>3.0879404047152215E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="47"/>
+    <row r="9" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="48"/>
       <c r="C9" s="4" t="s">
         <v>17</v>
       </c>
@@ -11012,8 +11012,8 @@
         <v>2.6567681351349553E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="47"/>
+    <row r="10" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="48"/>
       <c r="C10" s="4" t="s">
         <v>4</v>
       </c>
@@ -11082,8 +11082,8 @@
         <v>2.9035289801220693E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="47"/>
+    <row r="11" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="48"/>
       <c r="C11" s="4" t="s">
         <v>5</v>
       </c>
@@ -11152,8 +11152,8 @@
         <v>3.4742663735967461E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="48"/>
+    <row r="12" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="49"/>
       <c r="C12" s="6" t="s">
         <v>20</v>
       </c>
@@ -11222,8 +11222,8 @@
         <v>3.2014566755899074E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B13" s="55" t="s">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B13" s="45" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="25"/>
@@ -11244,8 +11244,8 @@
       <c r="R13" s="29"/>
       <c r="S13" s="34"/>
     </row>
-    <row r="14" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="47" t="s">
+    <row r="14" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="48" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -11316,8 +11316,8 @@
         <v>2.1166709549459383E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="47"/>
+    <row r="15" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="48"/>
       <c r="C15" s="4" t="s">
         <v>18</v>
       </c>
@@ -11386,8 +11386,8 @@
         <v>2.089825219249036E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="47"/>
+    <row r="16" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="48"/>
       <c r="C16" s="4" t="s">
         <v>3</v>
       </c>
@@ -11456,8 +11456,8 @@
         <v>1.3459823726881929E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="47"/>
+    <row r="17" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="48"/>
       <c r="C17" s="4" t="s">
         <v>19</v>
       </c>
@@ -11526,8 +11526,8 @@
         <v>1.1321681226052151E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="47"/>
+    <row r="18" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="48"/>
       <c r="C18" s="4" t="s">
         <v>17</v>
       </c>
@@ -11596,8 +11596,8 @@
         <v>2.1004350908505859E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="47"/>
+    <row r="19" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="48"/>
       <c r="C19" s="4" t="s">
         <v>4</v>
       </c>
@@ -11666,8 +11666,8 @@
         <v>1.7816473545345952E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="47"/>
+    <row r="20" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="48"/>
       <c r="C20" s="4" t="s">
         <v>5</v>
       </c>
@@ -11736,8 +11736,8 @@
         <v>9.4185790570313638E-3</v>
       </c>
     </row>
-    <row r="21" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="48"/>
+    <row r="21" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="49"/>
       <c r="C21" s="6" t="s">
         <v>20</v>
       </c>
@@ -11806,8 +11806,8 @@
         <v>1.9706496055853336E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B22" s="55" t="s">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B22" s="45" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="25"/>
@@ -11828,8 +11828,8 @@
       <c r="R22" s="29"/>
       <c r="S22" s="34"/>
     </row>
-    <row r="23" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="47" t="s">
+    <row r="23" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -11900,8 +11900,8 @@
         <v>4.4643017846348901E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="47"/>
+    <row r="24" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="48"/>
       <c r="C24" s="4" t="s">
         <v>18</v>
       </c>
@@ -11970,8 +11970,8 @@
         <v>3.997170768273773E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="47"/>
+    <row r="25" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="48"/>
       <c r="C25" s="4" t="s">
         <v>3</v>
       </c>
@@ -12040,8 +12040,8 @@
         <v>4.987208440938274E-2</v>
       </c>
     </row>
-    <row r="26" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="47"/>
+    <row r="26" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="48"/>
       <c r="C26" s="4" t="s">
         <v>19</v>
       </c>
@@ -12110,8 +12110,8 @@
         <v>3.8326001109827292E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="47"/>
+    <row r="27" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="48"/>
       <c r="C27" s="4" t="s">
         <v>17</v>
       </c>
@@ -12180,8 +12180,8 @@
         <v>3.6077666375167086E-2</v>
       </c>
     </row>
-    <row r="28" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="47"/>
+    <row r="28" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="48"/>
       <c r="C28" s="4" t="s">
         <v>4</v>
       </c>
@@ -12250,8 +12250,8 @@
         <v>3.9652799941969304E-2</v>
       </c>
     </row>
-    <row r="29" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="47"/>
+    <row r="29" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="48"/>
       <c r="C29" s="4" t="s">
         <v>5</v>
       </c>
@@ -12320,8 +12320,8 @@
         <v>4.4563019353375137E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="48"/>
+    <row r="30" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="49"/>
       <c r="C30" s="4" t="s">
         <v>20</v>
       </c>
@@ -12390,8 +12390,8 @@
         <v>4.853500899210151E-2</v>
       </c>
     </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B31" s="55" t="s">
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B31" s="45" t="s">
         <v>23</v>
       </c>
       <c r="C31" s="25"/>
@@ -12412,8 +12412,8 @@
       <c r="R31" s="29"/>
       <c r="S31" s="34"/>
     </row>
-    <row r="32" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="47" t="s">
+    <row r="32" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="48" t="s">
         <v>23</v>
       </c>
       <c r="C32" s="2" t="s">
@@ -12484,8 +12484,8 @@
         <v>4.0284146068368658E-2</v>
       </c>
     </row>
-    <row r="33" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="47"/>
+    <row r="33" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="48"/>
       <c r="C33" s="4" t="s">
         <v>18</v>
       </c>
@@ -12554,8 +12554,8 @@
         <v>3.621632839362391E-2</v>
       </c>
     </row>
-    <row r="34" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="47"/>
+    <row r="34" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="48"/>
       <c r="C34" s="4" t="s">
         <v>3</v>
       </c>
@@ -12624,8 +12624,8 @@
         <v>5.0893245309722293E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="47"/>
+    <row r="35" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="48"/>
       <c r="C35" s="4" t="s">
         <v>19</v>
       </c>
@@ -12694,8 +12694,8 @@
         <v>1.3929774849661306E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="47"/>
+    <row r="36" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="48"/>
       <c r="C36" s="4" t="s">
         <v>17</v>
       </c>
@@ -12764,8 +12764,8 @@
         <v>1.9587671820538728E-2</v>
       </c>
     </row>
-    <row r="37" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="47"/>
+    <row r="37" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="48"/>
       <c r="C37" s="4" t="s">
         <v>4</v>
       </c>
@@ -12834,8 +12834,8 @@
         <v>2.7874808831604404E-2</v>
       </c>
     </row>
-    <row r="38" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="47"/>
+    <row r="38" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="48"/>
       <c r="C38" s="4" t="s">
         <v>5</v>
       </c>
@@ -12904,8 +12904,8 @@
         <v>2.6347147377501812E-2</v>
       </c>
     </row>
-    <row r="39" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="48"/>
+    <row r="39" spans="2:19" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="49"/>
       <c r="C39" s="6" t="s">
         <v>20</v>
       </c>
@@ -12983,8 +12983,8 @@
     <mergeCell ref="B14:B21"/>
     <mergeCell ref="B23:B30"/>
   </mergeCells>
-  <conditionalFormatting sqref="D5 F5 H5 J5 L5 N5 P5 R5">
-    <cfRule type="colorScale" priority="40">
+  <conditionalFormatting sqref="D6 F6 H6 J6 L6 N6 P6 R6">
+    <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -12995,8 +12995,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7 F7 H7 J7 L7 N7 P7 R7">
-    <cfRule type="colorScale" priority="38">
+  <conditionalFormatting sqref="D11 F11 H11 J11 L11 N11 P11 R11">
+    <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -13007,8 +13007,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8 F8 H8 J8 L8 N8 P8 R8">
-    <cfRule type="colorScale" priority="37">
+  <conditionalFormatting sqref="D21 F21 H21 J21 L21 N21 P21 R21">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -13019,8 +13019,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D9 F9 H9 J9 L9 N9 P9 R9">
-    <cfRule type="colorScale" priority="36">
+  <conditionalFormatting sqref="D25 F25 H25 J25 L25 N25 P25 R25">
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -13031,8 +13031,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10 F10 H10 J10 L10 N10 P10 R10">
-    <cfRule type="colorScale" priority="35">
+  <conditionalFormatting sqref="D26 F26 H26 J26 L26 N26 P26 R26">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -13043,128 +13043,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D12 F12 H12 J12 L12 N12 P12 R12">
-    <cfRule type="colorScale" priority="33">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14 F14 H14 J14 L14 N14 P14 R14">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D15 F15 H15 J15 L15 N15 P15 R15">
-    <cfRule type="colorScale" priority="31">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D16 F16 H16 J16 L16 N16 P16 R16">
-    <cfRule type="colorScale" priority="30">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17 F17 H17 J17 L17 N17 P17 R17">
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D18 F18 H18 J18 L18 N18 P18 R18">
-    <cfRule type="colorScale" priority="28">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D19 F19 H19 J19 L19 N19 P19 R19">
-    <cfRule type="colorScale" priority="27">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D20 F20 H20 J20 L20 N20 P20 R20">
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D23 F23 H23 J23 L23 N23 P23 R23">
-    <cfRule type="colorScale" priority="24">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D24 F24 H24 J24 L24 N24 P24 R24">
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D28 F28 H28 J28 L28 N28 P28 R28">
-    <cfRule type="colorScale" priority="19">
+  <conditionalFormatting sqref="D27 F27 H27 J27 L27 N27 P27 R27">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -13187,7 +13067,259 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D33 F33 H33 J33 L33 N33 P33 R33">
+  <conditionalFormatting sqref="D32 F32 H32 J32 L32 N32 P32 R32">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35 F35 H35 J35 L35 N35 P35 R35">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36 F36 H36 J36 L36 N36 P36 R36">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38 F38 H38 J38 L38 N38 P38 R38">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39 F39 H39 J39 L39 N39 P39 R39">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5 D5 H5 J5 L5 N5 P5 R5">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7 D7 H7 J7 L7 N7 P7 R7">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8 D8 H8 J8 L8 N8 P8 R8">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9 D9 H9 J9 L9 N9 P9 R9">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10 D10 H10 J10 L10 N10 P10 R10">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12 D12 H12 J12 L12 N12 P12 R12">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14 D14 H14 J14 L14 N14 P14 R14">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15 D15 H15 J15 L15 N15 P15 R15">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16 D16 H16 J16 L16 N16 P16 R16">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F17 D17 H17 J17 L17 N17 P17 R17">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18 D18 H18 J18 L18 N18 P18 R18">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F19 D19 H19 J19 L19 N19 P19 R19">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20 D20 H20 J20 L20 N20 P20 R20">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F23 D23 H23 J23 L23 N23 P23 R23">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F24 D24 H24 J24 L24 N24 P24 R24">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F28 D28 H28 J28 L28 N28 P28 R28">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F33 D33 H33 J33 L33 N33 P33 R33">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -13199,7 +13331,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34 F34 H34 J34 L34 N34 P34 R34">
+  <conditionalFormatting sqref="F34 D34 H34 J34 L34 N34 P34 R34">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -13211,140 +13343,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37 F37 H37 J37 L37 N37 P37 R37">
+  <conditionalFormatting sqref="F37 D37 H37 J37 L37 N37 P37 R37">
     <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F6 D6 H6 J6 L6 N6 P6 R6">
-    <cfRule type="colorScale" priority="39">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F11 D11 H11 J11 L11 N11 P11 R11">
-    <cfRule type="colorScale" priority="34">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F21 D21 H21 J21 L21 N21 P21 R21">
-    <cfRule type="colorScale" priority="25">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F25 D25 H25 J25 L25 N25 P25 R25">
-    <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F26 D26 H26 J26 L26 N26 P26 R26">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F27 D27 H27 J27 L27 N27 P27 R27">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F32 D32 H32 J32 L32 N32 P32 R32">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F35 D35 H35 J35 L35 N35 P35 R35">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F36 D36 H36 J36 L36 N36 P36 R36">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F38 D38 H38 J38 L38 N38 P38 R38">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F39 D39 H39 J39 L39 N39 P39 R39">
-    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -13365,22 +13365,22 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="11" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" style="16" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" customWidth="1"/>
-    <col min="16" max="16" width="10.6640625" style="16" customWidth="1"/>
-    <col min="18" max="18" width="10.6640625" style="16" customWidth="1"/>
-    <col min="20" max="20" width="1.6640625" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="11" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="16" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" style="16" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" style="16" customWidth="1"/>
+    <col min="20" max="20" width="1.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:25" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:25" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="12" t="str">
         <f>IF(Wind_overview_classifier!B2=0,"",Wind_overview_classifier!B2)</f>
         <v/>
@@ -13389,80 +13389,80 @@
         <f>IF(Wind_overview_classifier!C2=0,"",Wind_overview_classifier!C2)</f>
         <v>Classifiers</v>
       </c>
-      <c r="D2" s="49" t="str">
+      <c r="D2" s="50" t="str">
         <f>IF(Wind_overview_classifier!D2=0,"",Wind_overview_classifier!D2)</f>
         <v>Augmented</v>
       </c>
-      <c r="E2" s="50" t="str">
+      <c r="E2" s="51" t="str">
         <f>IF(Aug_overview_classifier!E2=0,"",Aug_overview_classifier!E2)</f>
         <v/>
       </c>
-      <c r="F2" s="50" t="str">
+      <c r="F2" s="51" t="str">
         <f>IF(Aug_overview_classifier!F2=0,"",Aug_overview_classifier!F2)</f>
         <v/>
       </c>
-      <c r="G2" s="50" t="str">
+      <c r="G2" s="51" t="str">
         <f>IF(Aug_overview_classifier!G2=0,"",Aug_overview_classifier!G2)</f>
         <v/>
       </c>
-      <c r="H2" s="50" t="str">
+      <c r="H2" s="51" t="str">
         <f>IF(Aug_overview_classifier!H2=0,"",Aug_overview_classifier!H2)</f>
         <v/>
       </c>
-      <c r="I2" s="50" t="str">
+      <c r="I2" s="51" t="str">
         <f>IF(Aug_overview_classifier!I2=0,"",Aug_overview_classifier!I2)</f>
         <v/>
       </c>
-      <c r="J2" s="50" t="str">
+      <c r="J2" s="51" t="str">
         <f>IF(Aug_overview_classifier!J2=0,"",Aug_overview_classifier!J2)</f>
         <v/>
       </c>
-      <c r="K2" s="51" t="str">
+      <c r="K2" s="52" t="str">
         <f>IF(Aug_overview_classifier!K2=0,"",Aug_overview_classifier!K2)</f>
         <v/>
       </c>
-      <c r="L2" s="45" t="str">
+      <c r="L2" s="46" t="str">
         <f>IF(Wind_overview_classifier!L2=0,"",Wind_overview_classifier!L2)</f>
         <v>Windowed</v>
       </c>
-      <c r="M2" s="46" t="str">
+      <c r="M2" s="47" t="str">
         <f>IF(Aug_overview_classifier!M2=0,"",Aug_overview_classifier!M2)</f>
         <v/>
       </c>
-      <c r="N2" s="46" t="str">
+      <c r="N2" s="47" t="str">
         <f>IF(Aug_overview_classifier!N2=0,"",Aug_overview_classifier!N2)</f>
         <v/>
       </c>
-      <c r="O2" s="46" t="str">
+      <c r="O2" s="47" t="str">
         <f>IF(Aug_overview_classifier!O2=0,"",Aug_overview_classifier!O2)</f>
         <v/>
       </c>
-      <c r="P2" s="46" t="str">
+      <c r="P2" s="47" t="str">
         <f>IF(Aug_overview_classifier!P2=0,"",Aug_overview_classifier!P2)</f>
         <v/>
       </c>
-      <c r="Q2" s="46" t="str">
+      <c r="Q2" s="47" t="str">
         <f>IF(Aug_overview_classifier!Q2=0,"",Aug_overview_classifier!Q2)</f>
         <v/>
       </c>
-      <c r="R2" s="46" t="str">
+      <c r="R2" s="47" t="str">
         <f>IF(Aug_overview_classifier!R2=0,"",Aug_overview_classifier!R2)</f>
         <v/>
       </c>
-      <c r="S2" s="46" t="str">
+      <c r="S2" s="47" t="str">
         <f>IF(Aug_overview_classifier!S2=0,"",Aug_overview_classifier!S2)</f>
         <v/>
       </c>
-      <c r="U2" s="54" t="s">
+      <c r="U2" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="V2" s="54"/>
-      <c r="X2" s="54" t="s">
+      <c r="V2" s="55"/>
+      <c r="X2" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="Y2" s="54"/>
+      <c r="Y2" s="55"/>
     </row>
-    <row r="3" spans="2:25" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:25" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="35" t="str">
         <f>IF(Wind_overview_classifier!B3=0,"",Wind_overview_classifier!B3)</f>
         <v>Model</v>
@@ -13536,7 +13536,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B4" s="24" t="str">
         <f>IF(Wind_overview_classifier!B4=0,"",Wind_overview_classifier!B4)</f>
         <v>ESC10</v>
@@ -13610,8 +13610,8 @@
         <v>Std</v>
       </c>
     </row>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B5" s="53" t="str">
+    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B5" s="54" t="str">
         <f>IF(Wind_overview_classifier!B5=0,"",Wind_overview_classifier!B5)</f>
         <v>ESC10</v>
       </c>
@@ -13700,8 +13700,8 @@
         <v>-2.9738562091503495E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B6" s="47" t="str">
+    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B6" s="48" t="str">
         <f>IF(Aug_overview_classifier!B6=0,"",Aug_overview_classifier!B6)</f>
         <v/>
       </c>
@@ -13790,8 +13790,8 @@
         <v>-0.18308641975308693</v>
       </c>
     </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B7" s="47" t="str">
+    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B7" s="48" t="str">
         <f>IF(Aug_overview_classifier!B7=0,"",Aug_overview_classifier!B7)</f>
         <v/>
       </c>
@@ -13880,8 +13880,8 @@
         <v>-6.6782810685250382E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B8" s="47" t="str">
+    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B8" s="48" t="str">
         <f>IF(Aug_overview_classifier!B8=0,"",Aug_overview_classifier!B8)</f>
         <v/>
       </c>
@@ -13970,8 +13970,8 @@
         <v>-6.2133775566611704E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B9" s="47" t="str">
+    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B9" s="48" t="str">
         <f>IF(Aug_overview_classifier!B9=0,"",Aug_overview_classifier!B9)</f>
         <v/>
       </c>
@@ -14060,8 +14060,8 @@
         <v>-8.1578663211316793E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B10" s="47" t="str">
+    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B10" s="48" t="str">
         <f>IF(Aug_overview_classifier!B10=0,"",Aug_overview_classifier!B10)</f>
         <v/>
       </c>
@@ -14150,8 +14150,8 @@
         <v>-6.8330649490070283E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B11" s="47" t="str">
+    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B11" s="48" t="str">
         <f>IF(Aug_overview_classifier!B11=0,"",Aug_overview_classifier!B11)</f>
         <v/>
       </c>
@@ -14240,8 +14240,8 @@
         <v>-2.599286033021031E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B12" s="48" t="str">
+    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B12" s="49" t="str">
         <f>IF(Aug_overview_classifier!B12=0,"",Aug_overview_classifier!B12)</f>
         <v/>
       </c>
@@ -14330,7 +14330,7 @@
         <v>-1.3618233618233999E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B13" s="30" t="str">
         <f>IF(Wind_overview_classifier!B13=0,"",Wind_overview_classifier!B13)</f>
         <v>BDLib2</v>
@@ -14403,19 +14403,19 @@
         <f>IF(Wind_overview_classifier!S13=0,"",Wind_overview_classifier!S13)</f>
         <v/>
       </c>
-      <c r="U13" s="52">
+      <c r="U13" s="53">
         <f>AVERAGE(U5:V12)</f>
         <v>-7.9568010334686051E-2</v>
       </c>
-      <c r="V13" s="52"/>
-      <c r="X13" s="52">
+      <c r="V13" s="53"/>
+      <c r="X13" s="53">
         <f>AVERAGE(X5:Y12)</f>
         <v>-6.9913669799093039E-2</v>
       </c>
-      <c r="Y13" s="52"/>
+      <c r="Y13" s="53"/>
     </row>
-    <row r="14" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B14" s="53" t="str">
+    <row r="14" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B14" s="54" t="str">
         <f>IF(Wind_overview_classifier!B14=0,"",Wind_overview_classifier!B14)</f>
         <v>BDLib2</v>
       </c>
@@ -14504,8 +14504,8 @@
         <v>-6.6764132553606692E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B15" s="47" t="str">
+    <row r="15" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B15" s="48" t="str">
         <f>IF(Aug_overview_classifier!B15=0,"",Aug_overview_classifier!B15)</f>
         <v/>
       </c>
@@ -14594,8 +14594,8 @@
         <v>-0.19017543859649166</v>
       </c>
     </row>
-    <row r="16" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B16" s="47" t="str">
+    <row r="16" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B16" s="48" t="str">
         <f>IF(Aug_overview_classifier!B16=0,"",Aug_overview_classifier!B16)</f>
         <v/>
       </c>
@@ -14684,8 +14684,8 @@
         <v>2.0520050125313549E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B17" s="47" t="str">
+    <row r="17" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B17" s="48" t="str">
         <f>IF(Aug_overview_classifier!B17=0,"",Aug_overview_classifier!B17)</f>
         <v/>
       </c>
@@ -14774,8 +14774,8 @@
         <v>-5.7268170426065579E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B18" s="47" t="str">
+    <row r="18" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B18" s="48" t="str">
         <f>IF(Aug_overview_classifier!B18=0,"",Aug_overview_classifier!B18)</f>
         <v/>
       </c>
@@ -14864,8 +14864,8 @@
         <v>1.5587044534412842E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B19" s="47" t="str">
+    <row r="19" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B19" s="48" t="str">
         <f>IF(Aug_overview_classifier!B19=0,"",Aug_overview_classifier!B19)</f>
         <v/>
       </c>
@@ -14954,8 +14954,8 @@
         <v>-2.1577666794723949E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B20" s="47" t="str">
+    <row r="20" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B20" s="48" t="str">
         <f>IF(Aug_overview_classifier!B20=0,"",Aug_overview_classifier!B20)</f>
         <v/>
       </c>
@@ -15044,8 +15044,8 @@
         <v>0.11820534943917083</v>
       </c>
     </row>
-    <row r="21" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B21" s="48" t="str">
+    <row r="21" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B21" s="49" t="str">
         <f>IF(Aug_overview_classifier!B21=0,"",Aug_overview_classifier!B21)</f>
         <v/>
       </c>
@@ -15134,7 +15134,7 @@
         <v>0.19658521303258114</v>
       </c>
     </row>
-    <row r="22" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B22" s="30" t="str">
         <f>IF(Wind_overview_classifier!B22=0,"",Wind_overview_classifier!B22)</f>
         <v>US8K</v>
@@ -15207,19 +15207,19 @@
         <f>IF(Wind_overview_classifier!S22=0,"",Wind_overview_classifier!S22)</f>
         <v/>
       </c>
-      <c r="U22" s="52">
+      <c r="U22" s="53">
         <f>AVERAGE(U14:V21)</f>
         <v>-5.6429771014280435E-2</v>
       </c>
-      <c r="V22" s="52"/>
-      <c r="X22" s="52">
+      <c r="V22" s="53"/>
+      <c r="X22" s="53">
         <f>AVERAGE(X14:Y21)</f>
         <v>1.4009872496864445E-3</v>
       </c>
-      <c r="Y22" s="52"/>
+      <c r="Y22" s="53"/>
     </row>
-    <row r="23" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B23" s="53" t="str">
+    <row r="23" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B23" s="54" t="str">
         <f>IF(Wind_overview_classifier!B23=0,"",Wind_overview_classifier!B23)</f>
         <v>US8K</v>
       </c>
@@ -15308,8 +15308,8 @@
         <v>-7.3305794695187276E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B24" s="47" t="str">
+    <row r="24" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B24" s="48" t="str">
         <f>IF(Aug_overview_classifier!B24=0,"",Aug_overview_classifier!B24)</f>
         <v/>
       </c>
@@ -15398,8 +15398,8 @@
         <v>-0.19428799285871357</v>
       </c>
     </row>
-    <row r="25" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B25" s="47" t="str">
+    <row r="25" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B25" s="48" t="str">
         <f>IF(Aug_overview_classifier!B25=0,"",Aug_overview_classifier!B25)</f>
         <v/>
       </c>
@@ -15488,8 +15488,8 @@
         <v>-6.8259235188211864E-2</v>
       </c>
     </row>
-    <row r="26" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B26" s="47" t="str">
+    <row r="26" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B26" s="48" t="str">
         <f>IF(Aug_overview_classifier!B26=0,"",Aug_overview_classifier!B26)</f>
         <v/>
       </c>
@@ -15578,8 +15578,8 @@
         <v>-5.7821717769824699E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B27" s="47" t="str">
+    <row r="27" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B27" s="48" t="str">
         <f>IF(Aug_overview_classifier!B27=0,"",Aug_overview_classifier!B27)</f>
         <v/>
       </c>
@@ -15668,8 +15668,8 @@
         <v>-3.1772301279066273E-2</v>
       </c>
     </row>
-    <row r="28" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B28" s="47" t="str">
+    <row r="28" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B28" s="48" t="str">
         <f>IF(Aug_overview_classifier!B28=0,"",Aug_overview_classifier!B28)</f>
         <v/>
       </c>
@@ -15758,8 +15758,8 @@
         <v>-3.9738486748595259E-2</v>
       </c>
     </row>
-    <row r="29" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B29" s="47" t="str">
+    <row r="29" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B29" s="48" t="str">
         <f>IF(Aug_overview_classifier!B29=0,"",Aug_overview_classifier!B29)</f>
         <v/>
       </c>
@@ -15848,8 +15848,8 @@
         <v>-7.1847142469436576E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B30" s="48" t="str">
+    <row r="30" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B30" s="49" t="str">
         <f>IF(Aug_overview_classifier!B30=0,"",Aug_overview_classifier!B30)</f>
         <v/>
       </c>
@@ -15938,7 +15938,7 @@
         <v>-0.11535844087849767</v>
       </c>
     </row>
-    <row r="31" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B31" s="30" t="str">
         <f>IF(Wind_overview_classifier!B31=0,"",Wind_overview_classifier!B31)</f>
         <v>US8K_AV</v>
@@ -16011,19 +16011,19 @@
         <f>IF(Wind_overview_classifier!S31=0,"",Wind_overview_classifier!S31)</f>
         <v/>
       </c>
-      <c r="U31" s="52">
+      <c r="U31" s="53">
         <f>AVERAGE(U23:V30)</f>
         <v>-5.8828208236583648E-2</v>
       </c>
-      <c r="V31" s="52"/>
-      <c r="X31" s="52">
+      <c r="V31" s="53"/>
+      <c r="X31" s="53">
         <f>AVERAGE(X23:Y30)</f>
         <v>-7.2315381830499625E-2</v>
       </c>
-      <c r="Y31" s="52"/>
+      <c r="Y31" s="53"/>
     </row>
-    <row r="32" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B32" s="53" t="str">
+    <row r="32" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B32" s="54" t="str">
         <f>IF(Wind_overview_classifier!B32=0,"",Wind_overview_classifier!B32)</f>
         <v>US8K_AV</v>
       </c>
@@ -16112,8 +16112,8 @@
         <v>-5.2915939256235056E-2</v>
       </c>
     </row>
-    <row r="33" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B33" s="47" t="str">
+    <row r="33" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B33" s="48" t="str">
         <f>IF(Aug_overview_classifier!B33=0,"",Aug_overview_classifier!B33)</f>
         <v/>
       </c>
@@ -16202,8 +16202,8 @@
         <v>-6.2138101270161172E-2</v>
       </c>
     </row>
-    <row r="34" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B34" s="47" t="str">
+    <row r="34" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B34" s="48" t="str">
         <f>IF(Aug_overview_classifier!B34=0,"",Aug_overview_classifier!B34)</f>
         <v/>
       </c>
@@ -16292,8 +16292,8 @@
         <v>-4.9160061745109562E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B35" s="47" t="str">
+    <row r="35" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B35" s="48" t="str">
         <f>IF(Aug_overview_classifier!B35=0,"",Aug_overview_classifier!B35)</f>
         <v/>
       </c>
@@ -16382,8 +16382,8 @@
         <v>-5.4365459411869876E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B36" s="47" t="str">
+    <row r="36" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B36" s="48" t="str">
         <f>IF(Aug_overview_classifier!B36=0,"",Aug_overview_classifier!B36)</f>
         <v/>
       </c>
@@ -16472,8 +16472,8 @@
         <v>-3.9384666074033903E-2</v>
       </c>
     </row>
-    <row r="37" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B37" s="47" t="str">
+    <row r="37" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B37" s="48" t="str">
         <f>IF(Aug_overview_classifier!B37=0,"",Aug_overview_classifier!B37)</f>
         <v/>
       </c>
@@ -16562,8 +16562,8 @@
         <v>-3.7631188310879193E-2</v>
       </c>
     </row>
-    <row r="38" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B38" s="47" t="str">
+    <row r="38" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B38" s="48" t="str">
         <f>IF(Aug_overview_classifier!B38=0,"",Aug_overview_classifier!B38)</f>
         <v/>
       </c>
@@ -16652,8 +16652,8 @@
         <v>-7.3449125638510915E-2</v>
       </c>
     </row>
-    <row r="39" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B39" s="48" t="str">
+    <row r="39" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B39" s="49" t="str">
         <f>IF(Aug_overview_classifier!B39=0,"",Aug_overview_classifier!B39)</f>
         <v/>
       </c>
@@ -16742,17 +16742,17 @@
         <v>-4.8129389550780499E-2</v>
       </c>
     </row>
-    <row r="40" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="U40" s="52">
+    <row r="40" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="U40" s="53">
         <f>AVERAGE(U32:V39)</f>
         <v>-4.4885044745957267E-2</v>
       </c>
-      <c r="V40" s="52"/>
-      <c r="X40" s="52">
+      <c r="V40" s="53"/>
+      <c r="X40" s="53">
         <f>AVERAGE(X32:Y39)</f>
         <v>-5.5470411486258274E-2</v>
       </c>
-      <c r="Y40" s="52"/>
+      <c r="Y40" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="16">

</xml_diff>